<commit_message>
점검문서 sort > server추가
</commit_message>
<xml_diff>
--- a/이벤트DATA_KR.xlsx
+++ b/이벤트DATA_KR.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://webzen-my.sharepoint.com/personal/mssung_webzen_com/Documents/자동문서생성-20210014i1/r2mAutoMakeCL/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="227" documentId="13_ncr:1_{0FD6ADB6-7B08-4CF7-B47D-28D24761C236}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8A946AC5-E5D2-4F7F-8231-626E125CA4D3}"/>
+  <xr:revisionPtr revIDLastSave="232" documentId="13_ncr:1_{0FD6ADB6-7B08-4CF7-B47D-28D24761C236}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F096F6EB-10DA-4644-90A4-9FC28BCAB55D}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6F2C3106-E9E5-4E5A-A43E-54D895F8835E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$O$116</definedName>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="187">
   <si>
     <t>계정당 1회</t>
   </si>
@@ -593,6 +594,69 @@
   <si>
     <t>ItemID_1</t>
     <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>상급 변신 뽑기권[11회][귀속] X 6</t>
+  </si>
+  <si>
+    <t>희귀 변신 확정 뽑기권 조각[귀속] X 1</t>
+  </si>
+  <si>
+    <t>전리품 상자 제작서[귀속] X 11</t>
+  </si>
+  <si>
+    <t>상급 매터리얼 상자[귀속] X 1</t>
+  </si>
+  <si>
+    <t>희귀 포인트 충전석 상자[귀속] X 2</t>
+  </si>
+  <si>
+    <t>장비 각인석[귀속] X 10</t>
+  </si>
+  <si>
+    <t>최상급 특수 매터리얼 상자[귀속] X 1</t>
+  </si>
+  <si>
+    <t>상급 변신 뽑기권[11회][귀속] X 2</t>
+  </si>
+  <si>
+    <t>희귀 서번트 확정 뽑기권 조각[귀속] X 1</t>
+  </si>
+  <si>
+    <t>희귀 포인트 충전석 상자[귀속] X 3</t>
+  </si>
+  <si>
+    <t>상급 서번트 뽑기권[11회][귀속] X 2</t>
+  </si>
+  <si>
+    <t>상급 서번트 뽑기권[11회][귀속] X2</t>
+  </si>
+  <si>
+    <t>영웅 포인트 충전석 상자[귀속] X 2</t>
+  </si>
+  <si>
+    <t>영웅 포인트 충전석 상자[귀속] X 3</t>
+  </si>
+  <si>
+    <t>상급 서번트 뽑기권[11회][귀속] X 3</t>
+  </si>
+  <si>
+    <t>상급 변신 뽑기권[11회][귀속] X 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">전리품 상자 제작서[귀속] X 22 </t>
+  </si>
+  <si>
+    <t>상급 서번트 뽑기권[11회][귀속] X 6</t>
+  </si>
+  <si>
+    <t>타나토스의 강림[귀속] X 1</t>
+  </si>
+  <si>
+    <t>경험치 상승 매터리얼[이벤트][귀속] X 1</t>
+  </si>
+  <si>
+    <t>전리품 상자 제작서[귀속] X 22</t>
   </si>
 </sst>
 </file>
@@ -602,7 +666,7 @@
   <numFmts count="1">
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -686,8 +750,16 @@
       <charset val="129"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -705,8 +777,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="7">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -792,6 +870,34 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -852,7 +958,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -903,6 +1009,12 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="21">
@@ -1243,7 +1355,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C22" sqref="C22"/>
+      <selection pane="bottomLeft" activeCell="I28" sqref="I28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
@@ -4092,6 +4204,282 @@
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83A6365E-0AE6-4708-9D82-DAB22957BDFB}">
+  <sheetPr codeName="Sheet2"/>
+  <dimension ref="A1:B32"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="2" width="30.25" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="17" t="s">
+        <v>166</v>
+      </c>
+      <c r="B1" s="17" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="17" t="s">
+        <v>167</v>
+      </c>
+      <c r="B2" s="17" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="17" t="s">
+        <v>168</v>
+      </c>
+      <c r="B3" s="17" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" s="17" t="s">
+        <v>167</v>
+      </c>
+      <c r="B4" s="17" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="17" t="s">
+        <v>169</v>
+      </c>
+      <c r="B5" s="17" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" s="17" t="s">
+        <v>170</v>
+      </c>
+      <c r="B6" s="17" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" s="17" t="s">
+        <v>171</v>
+      </c>
+      <c r="B7" s="17" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" s="17" t="s">
+        <v>172</v>
+      </c>
+      <c r="B8" s="17" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" s="17" t="s">
+        <v>173</v>
+      </c>
+      <c r="B9" s="17" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="B10" s="17" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" s="17" t="s">
+        <v>169</v>
+      </c>
+      <c r="B11" s="17" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="B12" s="17" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="B13" s="17" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="B14" s="17" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" s="17" t="s">
+        <v>173</v>
+      </c>
+      <c r="B15" s="17" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" s="17" t="s">
+        <v>168</v>
+      </c>
+      <c r="B16" s="17" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" s="17" t="s">
+        <v>177</v>
+      </c>
+      <c r="B17" s="17" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" s="17" t="s">
+        <v>169</v>
+      </c>
+      <c r="B18" s="17" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="B19" s="17" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" s="17" t="s">
+        <v>167</v>
+      </c>
+      <c r="B20" s="17" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" s="17" t="s">
+        <v>168</v>
+      </c>
+      <c r="B21" s="17" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="B22" s="17" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A23" s="17" t="s">
+        <v>171</v>
+      </c>
+      <c r="B23" s="17" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A24" s="17" t="s">
+        <v>179</v>
+      </c>
+      <c r="B24" s="17" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A25" s="17" t="s">
+        <v>168</v>
+      </c>
+      <c r="B25" s="17" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A26" s="17" t="s">
+        <v>169</v>
+      </c>
+      <c r="B26" s="17" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A27" s="17" t="s">
+        <v>173</v>
+      </c>
+      <c r="B27" s="17" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A28" s="17" t="s">
+        <v>180</v>
+      </c>
+      <c r="B28" s="17" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A29" s="17" t="s">
+        <v>167</v>
+      </c>
+      <c r="B29" s="17" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A30" s="17" t="s">
+        <v>181</v>
+      </c>
+      <c r="B30" s="17" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A31" s="17" t="s">
+        <v>182</v>
+      </c>
+      <c r="B31" s="17" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A32" s="18" t="s">
+        <v>183</v>
+      </c>
+      <c r="B32" s="17" t="s">
+        <v>183</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
category > str 형 지정하여 추출
</commit_message>
<xml_diff>
--- a/이벤트DATA_KR.xlsx
+++ b/이벤트DATA_KR.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26605"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr codeName="현재_통합_문서" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://webzen.sharepoint.com/sites/R2M/Shared Documents/R2M전용도구/유료상점CL생성기/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="145" documentId="13_ncr:81_{AB671696-D832-4E10-BC32-0B2BF60F630D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{010FCF94-F673-4206-93F3-BF016D1443E7}"/>
+  <xr:revisionPtr revIDLastSave="147" documentId="13_ncr:81_{AB671696-D832-4E10-BC32-0B2BF60F630D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{156497D8-FCA3-4743-9FB1-391E5C53F2F0}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="2" xr2:uid="{6F2C3106-E9E5-4E5A-A43E-54D895F8835E}"/>
+    <workbookView xWindow="30840" yWindow="795" windowWidth="22500" windowHeight="14115" firstSheet="1" activeTab="2" xr2:uid="{6F2C3106-E9E5-4E5A-A43E-54D895F8835E}"/>
   </bookViews>
   <sheets>
     <sheet name="사용법" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'230223 업데이트'!$B$1:$Q$116</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'230330 업데이트'!$B$1:$O$56</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'230427 업데이트'!$B$1:$P$58</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'230427 업데이트'!$B$1:$T$58</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'230525 업데이트'!$B$1:$P$76</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">사용법!$H$1:$Y$46</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">템플릿!$B$1:$P$58</definedName>
@@ -1183,7 +1183,7 @@
   <numFmts count="1">
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
-  <fonts count="12">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1906,7 +1906,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 테마">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -2209,12 +2209,12 @@
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="7" ySplit="1" topLeftCell="I2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight"/>
+      <selection pane="bottomLeft"/>
       <selection pane="bottomRight" activeCell="J36" sqref="J36"/>
-      <selection pane="bottomLeft"/>
-      <selection pane="topRight"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="7" width="9" style="8"/>
     <col min="8" max="8" width="11.125" style="8" customWidth="1"/>
@@ -2234,7 +2234,7 @@
     <col min="22" max="16384" width="9" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="7:25" ht="16.5">
+    <row r="1" spans="7:25" ht="16.5" x14ac:dyDescent="0.3">
       <c r="G1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2285,7 +2285,7 @@
       <c r="X1"/>
       <c r="Y1"/>
     </row>
-    <row r="2" spans="7:25" ht="16.5" customHeight="1">
+    <row r="2" spans="7:25" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H2" s="5">
         <v>150</v>
       </c>
@@ -2325,7 +2325,7 @@
       <c r="X2"/>
       <c r="Y2"/>
     </row>
-    <row r="3" spans="7:25" ht="16.5">
+    <row r="3" spans="7:25" ht="16.5" x14ac:dyDescent="0.3">
       <c r="H3" s="5"/>
       <c r="I3" s="5"/>
       <c r="J3" s="5"/>
@@ -2351,7 +2351,7 @@
       <c r="X3"/>
       <c r="Y3"/>
     </row>
-    <row r="4" spans="7:25" ht="16.5">
+    <row r="4" spans="7:25" ht="16.5" x14ac:dyDescent="0.3">
       <c r="H4" s="5"/>
       <c r="I4" s="5"/>
       <c r="J4" s="5"/>
@@ -2377,7 +2377,7 @@
       <c r="X4"/>
       <c r="Y4"/>
     </row>
-    <row r="5" spans="7:25" ht="16.5">
+    <row r="5" spans="7:25" ht="16.5" x14ac:dyDescent="0.3">
       <c r="H5" s="5"/>
       <c r="I5" s="5"/>
       <c r="J5" s="5"/>
@@ -2403,7 +2403,7 @@
       <c r="X5"/>
       <c r="Y5"/>
     </row>
-    <row r="6" spans="7:25" ht="16.5">
+    <row r="6" spans="7:25" ht="16.5" x14ac:dyDescent="0.3">
       <c r="H6" s="5"/>
       <c r="I6" s="5"/>
       <c r="J6" s="5"/>
@@ -2429,7 +2429,7 @@
       <c r="X6"/>
       <c r="Y6"/>
     </row>
-    <row r="7" spans="7:25" ht="16.5">
+    <row r="7" spans="7:25" ht="16.5" x14ac:dyDescent="0.3">
       <c r="H7" s="5"/>
       <c r="I7" s="5"/>
       <c r="J7" s="5"/>
@@ -2455,7 +2455,7 @@
       <c r="X7"/>
       <c r="Y7"/>
     </row>
-    <row r="8" spans="7:25" ht="16.5">
+    <row r="8" spans="7:25" ht="16.5" x14ac:dyDescent="0.3">
       <c r="H8" s="5"/>
       <c r="I8" s="5"/>
       <c r="J8" s="5"/>
@@ -2481,7 +2481,7 @@
       <c r="X8"/>
       <c r="Y8"/>
     </row>
-    <row r="9" spans="7:25" ht="16.5">
+    <row r="9" spans="7:25" ht="16.5" x14ac:dyDescent="0.3">
       <c r="H9" s="5"/>
       <c r="I9" s="5"/>
       <c r="J9" s="5"/>
@@ -2507,7 +2507,7 @@
       <c r="X9"/>
       <c r="Y9"/>
     </row>
-    <row r="10" spans="7:25" ht="16.5">
+    <row r="10" spans="7:25" ht="16.5" x14ac:dyDescent="0.3">
       <c r="H10" s="5"/>
       <c r="I10" s="5"/>
       <c r="J10" s="5"/>
@@ -2533,7 +2533,7 @@
       <c r="X10"/>
       <c r="Y10"/>
     </row>
-    <row r="11" spans="7:25" ht="16.5">
+    <row r="11" spans="7:25" ht="16.5" x14ac:dyDescent="0.3">
       <c r="H11" s="7"/>
       <c r="I11" s="7"/>
       <c r="J11" s="7"/>
@@ -2559,7 +2559,7 @@
       <c r="X11"/>
       <c r="Y11"/>
     </row>
-    <row r="12" spans="7:25" ht="16.5">
+    <row r="12" spans="7:25" ht="16.5" x14ac:dyDescent="0.3">
       <c r="H12" s="7">
         <v>370</v>
       </c>
@@ -2601,7 +2601,7 @@
       <c r="X12"/>
       <c r="Y12"/>
     </row>
-    <row r="13" spans="7:25" ht="16.5">
+    <row r="13" spans="7:25" ht="16.5" x14ac:dyDescent="0.3">
       <c r="H13" s="7"/>
       <c r="I13" s="5"/>
       <c r="J13" s="7"/>
@@ -2629,7 +2629,7 @@
       <c r="X13"/>
       <c r="Y13"/>
     </row>
-    <row r="14" spans="7:25" ht="16.5">
+    <row r="14" spans="7:25" ht="16.5" x14ac:dyDescent="0.3">
       <c r="H14" s="7"/>
       <c r="I14" s="5"/>
       <c r="J14" s="7"/>
@@ -2657,7 +2657,7 @@
       <c r="X14"/>
       <c r="Y14"/>
     </row>
-    <row r="15" spans="7:25" ht="16.5">
+    <row r="15" spans="7:25" ht="16.5" x14ac:dyDescent="0.3">
       <c r="H15" s="7"/>
       <c r="I15" s="5"/>
       <c r="J15" s="7"/>
@@ -2685,7 +2685,7 @@
       <c r="X15"/>
       <c r="Y15"/>
     </row>
-    <row r="16" spans="7:25" ht="16.5">
+    <row r="16" spans="7:25" ht="16.5" x14ac:dyDescent="0.3">
       <c r="H16" s="7"/>
       <c r="I16" s="5"/>
       <c r="J16" s="7"/>
@@ -2713,7 +2713,7 @@
       <c r="X16"/>
       <c r="Y16"/>
     </row>
-    <row r="17" spans="8:25" ht="16.5">
+    <row r="17" spans="8:25" ht="16.5" x14ac:dyDescent="0.3">
       <c r="H17" s="7"/>
       <c r="I17" s="5"/>
       <c r="J17" s="7"/>
@@ -2741,7 +2741,7 @@
       <c r="X17"/>
       <c r="Y17"/>
     </row>
-    <row r="18" spans="8:25" ht="16.5">
+    <row r="18" spans="8:25" ht="16.5" x14ac:dyDescent="0.3">
       <c r="H18" s="7"/>
       <c r="I18" s="5"/>
       <c r="J18" s="7"/>
@@ -2769,7 +2769,7 @@
       <c r="X18"/>
       <c r="Y18"/>
     </row>
-    <row r="19" spans="8:25" s="20" customFormat="1" ht="16.5">
+    <row r="19" spans="8:25" s="20" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
       <c r="H19" s="21">
         <v>371</v>
       </c>
@@ -2811,7 +2811,7 @@
       <c r="X19" s="25"/>
       <c r="Y19" s="25"/>
     </row>
-    <row r="20" spans="8:25" s="20" customFormat="1" ht="16.5">
+    <row r="20" spans="8:25" s="20" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
       <c r="H20" s="21"/>
       <c r="I20" s="22"/>
       <c r="J20" s="21"/>
@@ -2839,7 +2839,7 @@
       <c r="X20" s="25"/>
       <c r="Y20" s="25"/>
     </row>
-    <row r="21" spans="8:25" s="20" customFormat="1" ht="16.5">
+    <row r="21" spans="8:25" s="20" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
       <c r="H21" s="21"/>
       <c r="I21" s="21"/>
       <c r="J21" s="21"/>
@@ -2867,7 +2867,7 @@
       <c r="X21" s="25"/>
       <c r="Y21" s="25"/>
     </row>
-    <row r="22" spans="8:25" s="20" customFormat="1" ht="16.5">
+    <row r="22" spans="8:25" s="20" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
       <c r="H22" s="21"/>
       <c r="I22" s="21"/>
       <c r="J22" s="21"/>
@@ -2895,7 +2895,7 @@
       <c r="X22" s="25"/>
       <c r="Y22" s="25"/>
     </row>
-    <row r="23" spans="8:25" s="20" customFormat="1" ht="16.5">
+    <row r="23" spans="8:25" s="20" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
       <c r="H23" s="21"/>
       <c r="I23" s="21"/>
       <c r="J23" s="21"/>
@@ -2923,7 +2923,7 @@
       <c r="X23" s="25"/>
       <c r="Y23" s="25"/>
     </row>
-    <row r="24" spans="8:25" s="20" customFormat="1" ht="16.5">
+    <row r="24" spans="8:25" s="20" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
       <c r="H24" s="21"/>
       <c r="I24" s="21"/>
       <c r="J24" s="21"/>
@@ -2951,7 +2951,7 @@
       <c r="X24" s="25"/>
       <c r="Y24" s="25"/>
     </row>
-    <row r="25" spans="8:25" s="20" customFormat="1" ht="16.5">
+    <row r="25" spans="8:25" s="20" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
       <c r="H25" s="21"/>
       <c r="I25" s="21"/>
       <c r="J25" s="21"/>
@@ -2979,7 +2979,7 @@
       <c r="X25" s="25"/>
       <c r="Y25" s="25"/>
     </row>
-    <row r="26" spans="8:25" ht="16.5">
+    <row r="26" spans="8:25" ht="16.5" x14ac:dyDescent="0.3">
       <c r="H26" s="7">
         <v>30012</v>
       </c>
@@ -3017,7 +3017,7 @@
       <c r="X26"/>
       <c r="Y26"/>
     </row>
-    <row r="27" spans="8:25" s="20" customFormat="1" ht="16.5">
+    <row r="27" spans="8:25" s="20" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
       <c r="H27" s="21">
         <v>20008</v>
       </c>
@@ -3057,7 +3057,7 @@
       <c r="X27" s="25"/>
       <c r="Y27" s="25"/>
     </row>
-    <row r="28" spans="8:25" s="20" customFormat="1" ht="16.5">
+    <row r="28" spans="8:25" s="20" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
       <c r="H28" s="21"/>
       <c r="I28" s="21"/>
       <c r="J28" s="26"/>
@@ -3085,7 +3085,7 @@
       <c r="X28" s="25"/>
       <c r="Y28" s="25"/>
     </row>
-    <row r="29" spans="8:25" s="20" customFormat="1" ht="16.5">
+    <row r="29" spans="8:25" s="20" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
       <c r="H29" s="21"/>
       <c r="I29" s="21"/>
       <c r="J29" s="21"/>
@@ -3113,7 +3113,7 @@
       <c r="X29" s="25"/>
       <c r="Y29" s="25"/>
     </row>
-    <row r="30" spans="8:25" s="20" customFormat="1" ht="16.5">
+    <row r="30" spans="8:25" s="20" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
       <c r="H30" s="21"/>
       <c r="I30" s="21"/>
       <c r="J30" s="21"/>
@@ -3141,7 +3141,7 @@
       <c r="X30" s="25"/>
       <c r="Y30" s="25"/>
     </row>
-    <row r="31" spans="8:25" s="20" customFormat="1" ht="16.5">
+    <row r="31" spans="8:25" s="20" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
       <c r="H31" s="21"/>
       <c r="I31" s="21"/>
       <c r="J31" s="21"/>
@@ -3169,7 +3169,7 @@
       <c r="X31" s="25"/>
       <c r="Y31" s="25"/>
     </row>
-    <row r="32" spans="8:25" s="20" customFormat="1" ht="16.5">
+    <row r="32" spans="8:25" s="20" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
       <c r="H32" s="21"/>
       <c r="I32" s="21"/>
       <c r="J32" s="21"/>
@@ -3197,7 +3197,7 @@
       <c r="X32" s="25"/>
       <c r="Y32" s="25"/>
     </row>
-    <row r="33" spans="8:25" s="20" customFormat="1" ht="16.5">
+    <row r="33" spans="8:25" s="20" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
       <c r="H33" s="21"/>
       <c r="I33" s="21"/>
       <c r="J33" s="26"/>
@@ -3225,7 +3225,7 @@
       <c r="X33" s="25"/>
       <c r="Y33" s="25"/>
     </row>
-    <row r="34" spans="8:25" s="20" customFormat="1" ht="16.5">
+    <row r="34" spans="8:25" s="20" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
       <c r="H34" s="21"/>
       <c r="I34" s="21"/>
       <c r="J34" s="26"/>
@@ -3253,7 +3253,7 @@
       <c r="X34" s="25"/>
       <c r="Y34" s="25"/>
     </row>
-    <row r="35" spans="8:25" ht="16.5">
+    <row r="35" spans="8:25" ht="16.5" x14ac:dyDescent="0.3">
       <c r="H35" s="7">
         <v>1104</v>
       </c>
@@ -3291,7 +3291,7 @@
       <c r="X35"/>
       <c r="Y35"/>
     </row>
-    <row r="36" spans="8:25" ht="16.5">
+    <row r="36" spans="8:25" ht="16.5" x14ac:dyDescent="0.3">
       <c r="H36" s="7"/>
       <c r="I36" s="7"/>
       <c r="J36" s="12"/>
@@ -3315,7 +3315,7 @@
       <c r="X36"/>
       <c r="Y36"/>
     </row>
-    <row r="37" spans="8:25" ht="16.5">
+    <row r="37" spans="8:25" ht="16.5" x14ac:dyDescent="0.3">
       <c r="H37" s="7"/>
       <c r="I37" s="7"/>
       <c r="J37" s="12"/>
@@ -3339,7 +3339,7 @@
       <c r="X37"/>
       <c r="Y37"/>
     </row>
-    <row r="38" spans="8:25" ht="16.5">
+    <row r="38" spans="8:25" ht="16.5" x14ac:dyDescent="0.3">
       <c r="H38" s="7"/>
       <c r="I38" s="7"/>
       <c r="J38" s="12"/>
@@ -3363,7 +3363,7 @@
       <c r="X38"/>
       <c r="Y38"/>
     </row>
-    <row r="39" spans="8:25" ht="16.5">
+    <row r="39" spans="8:25" ht="16.5" x14ac:dyDescent="0.3">
       <c r="H39" s="7"/>
       <c r="I39" s="7"/>
       <c r="J39" s="12"/>
@@ -3387,7 +3387,7 @@
       <c r="X39"/>
       <c r="Y39"/>
     </row>
-    <row r="40" spans="8:25" ht="16.5">
+    <row r="40" spans="8:25" ht="16.5" x14ac:dyDescent="0.3">
       <c r="H40" s="7"/>
       <c r="I40" s="7"/>
       <c r="J40" s="12"/>
@@ -3411,7 +3411,7 @@
       <c r="X40"/>
       <c r="Y40"/>
     </row>
-    <row r="41" spans="8:25" s="20" customFormat="1" ht="16.5">
+    <row r="41" spans="8:25" s="20" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
       <c r="H41" s="21">
         <v>1105</v>
       </c>
@@ -3449,7 +3449,7 @@
       <c r="X41" s="25"/>
       <c r="Y41" s="25"/>
     </row>
-    <row r="42" spans="8:25" s="20" customFormat="1" ht="16.5">
+    <row r="42" spans="8:25" s="20" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
       <c r="H42" s="21"/>
       <c r="I42" s="21"/>
       <c r="J42" s="26"/>
@@ -3473,7 +3473,7 @@
       <c r="X42" s="25"/>
       <c r="Y42" s="25"/>
     </row>
-    <row r="43" spans="8:25" s="20" customFormat="1" ht="16.5">
+    <row r="43" spans="8:25" s="20" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
       <c r="H43" s="21"/>
       <c r="I43" s="21"/>
       <c r="J43" s="26"/>
@@ -3497,7 +3497,7 @@
       <c r="X43" s="25"/>
       <c r="Y43" s="25"/>
     </row>
-    <row r="44" spans="8:25" s="20" customFormat="1" ht="16.5">
+    <row r="44" spans="8:25" s="20" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
       <c r="H44" s="21"/>
       <c r="I44" s="21"/>
       <c r="J44" s="26"/>
@@ -3521,7 +3521,7 @@
       <c r="X44" s="25"/>
       <c r="Y44" s="25"/>
     </row>
-    <row r="45" spans="8:25" s="20" customFormat="1" ht="16.5">
+    <row r="45" spans="8:25" s="20" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
       <c r="H45" s="21"/>
       <c r="I45" s="21"/>
       <c r="J45" s="21"/>
@@ -3545,7 +3545,7 @@
       <c r="X45" s="25"/>
       <c r="Y45" s="25"/>
     </row>
-    <row r="46" spans="8:25" s="20" customFormat="1" ht="16.5">
+    <row r="46" spans="8:25" s="20" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
       <c r="H46" s="21"/>
       <c r="I46" s="21"/>
       <c r="J46" s="21"/>
@@ -3577,7 +3577,7 @@
       <selection pane="bottomRight" activeCell="K7" sqref="K7"/>
       <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
       <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
-      <autoFilter ref="H1:Y46" xr:uid="{FD9B61D1-F8B0-4FAF-B190-93EA59887337}"/>
+      <autoFilter ref="H1:Y46" xr:uid="{D0406083-7B07-4048-9F1C-EE6E949823B9}"/>
     </customSheetView>
   </customSheetViews>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -3594,12 +3594,12 @@
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight"/>
+      <selection pane="bottomLeft"/>
       <selection pane="bottomRight" activeCell="D27" sqref="D27"/>
-      <selection pane="bottomLeft"/>
-      <selection pane="topRight"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="10.25" style="34" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.125" style="8" customWidth="1"/>
@@ -3620,7 +3620,7 @@
     <col min="17" max="16384" width="9" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="16.5">
+    <row r="1" spans="1:20" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A1" s="36" t="s">
         <v>0</v>
       </c>
@@ -3674,7 +3674,7 @@
       <c r="S1"/>
       <c r="T1"/>
     </row>
-    <row r="2" spans="1:20" ht="16.5" customHeight="1">
+    <row r="2" spans="1:20" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B2" s="5">
         <v>154</v>
       </c>
@@ -3719,7 +3719,7 @@
       <c r="S2"/>
       <c r="T2"/>
     </row>
-    <row r="3" spans="1:20" ht="16.5">
+    <row r="3" spans="1:20" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B3" s="5"/>
       <c r="C3" s="5"/>
       <c r="D3" s="5"/>
@@ -3750,7 +3750,7 @@
       <c r="S3"/>
       <c r="T3"/>
     </row>
-    <row r="4" spans="1:20" ht="16.5">
+    <row r="4" spans="1:20" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B4" s="5"/>
       <c r="C4" s="5"/>
       <c r="D4" s="5"/>
@@ -3781,7 +3781,7 @@
       <c r="S4"/>
       <c r="T4"/>
     </row>
-    <row r="5" spans="1:20" ht="16.5">
+    <row r="5" spans="1:20" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B5" s="5"/>
       <c r="C5" s="5"/>
       <c r="D5" s="5"/>
@@ -3812,7 +3812,7 @@
       <c r="S5"/>
       <c r="T5"/>
     </row>
-    <row r="6" spans="1:20" ht="16.5">
+    <row r="6" spans="1:20" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
@@ -3843,7 +3843,7 @@
       <c r="S6"/>
       <c r="T6"/>
     </row>
-    <row r="7" spans="1:20" ht="16.5">
+    <row r="7" spans="1:20" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>
       <c r="D7" s="5"/>
@@ -3874,7 +3874,7 @@
       <c r="S7"/>
       <c r="T7"/>
     </row>
-    <row r="8" spans="1:20" ht="16.5">
+    <row r="8" spans="1:20" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B8" s="5"/>
       <c r="C8" s="5"/>
       <c r="D8" s="5"/>
@@ -3905,7 +3905,7 @@
       <c r="S8"/>
       <c r="T8"/>
     </row>
-    <row r="9" spans="1:20" ht="16.5">
+    <row r="9" spans="1:20" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B9" s="5"/>
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
@@ -3936,7 +3936,7 @@
       <c r="S9"/>
       <c r="T9"/>
     </row>
-    <row r="10" spans="1:20" ht="16.5">
+    <row r="10" spans="1:20" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B10" s="5"/>
       <c r="C10" s="5"/>
       <c r="D10" s="5"/>
@@ -3967,7 +3967,7 @@
       <c r="S10"/>
       <c r="T10"/>
     </row>
-    <row r="11" spans="1:20" ht="16.5">
+    <row r="11" spans="1:20" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B11" s="7"/>
       <c r="C11" s="7"/>
       <c r="D11" s="7"/>
@@ -3998,7 +3998,7 @@
       <c r="S11"/>
       <c r="T11"/>
     </row>
-    <row r="12" spans="1:20" ht="16.5">
+    <row r="12" spans="1:20" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B12" s="7">
         <v>156</v>
       </c>
@@ -4043,7 +4043,7 @@
       <c r="S12"/>
       <c r="T12"/>
     </row>
-    <row r="13" spans="1:20" ht="16.5">
+    <row r="13" spans="1:20" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B13" s="7"/>
       <c r="C13" s="7"/>
       <c r="D13" s="7"/>
@@ -4074,7 +4074,7 @@
       <c r="S13"/>
       <c r="T13"/>
     </row>
-    <row r="14" spans="1:20" ht="16.5">
+    <row r="14" spans="1:20" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B14" s="7"/>
       <c r="C14" s="7"/>
       <c r="D14" s="7"/>
@@ -4105,7 +4105,7 @@
       <c r="S14"/>
       <c r="T14"/>
     </row>
-    <row r="15" spans="1:20" ht="16.5">
+    <row r="15" spans="1:20" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B15" s="7"/>
       <c r="C15" s="7"/>
       <c r="D15" s="7"/>
@@ -4136,7 +4136,7 @@
       <c r="S15"/>
       <c r="T15"/>
     </row>
-    <row r="16" spans="1:20" ht="16.5">
+    <row r="16" spans="1:20" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B16" s="7"/>
       <c r="C16" s="7"/>
       <c r="D16" s="7"/>
@@ -4167,7 +4167,7 @@
       <c r="S16"/>
       <c r="T16"/>
     </row>
-    <row r="17" spans="2:20" ht="16.5">
+    <row r="17" spans="2:20" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B17" s="7"/>
       <c r="C17" s="7"/>
       <c r="D17" s="7"/>
@@ -4198,7 +4198,7 @@
       <c r="S17"/>
       <c r="T17"/>
     </row>
-    <row r="18" spans="2:20" ht="16.5">
+    <row r="18" spans="2:20" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B18" s="7"/>
       <c r="C18" s="7"/>
       <c r="D18" s="7"/>
@@ -4229,7 +4229,7 @@
       <c r="S18"/>
       <c r="T18"/>
     </row>
-    <row r="19" spans="2:20" ht="16.5">
+    <row r="19" spans="2:20" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B19" s="7"/>
       <c r="C19" s="7"/>
       <c r="D19" s="7"/>
@@ -4260,7 +4260,7 @@
       <c r="S19"/>
       <c r="T19"/>
     </row>
-    <row r="20" spans="2:20" ht="16.5">
+    <row r="20" spans="2:20" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B20" s="7"/>
       <c r="C20" s="7"/>
       <c r="D20" s="7"/>
@@ -4291,7 +4291,7 @@
       <c r="S20"/>
       <c r="T20"/>
     </row>
-    <row r="21" spans="2:20" ht="16.5">
+    <row r="21" spans="2:20" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B21" s="7"/>
       <c r="C21" s="7"/>
       <c r="D21" s="7"/>
@@ -4322,7 +4322,7 @@
       <c r="S21"/>
       <c r="T21"/>
     </row>
-    <row r="22" spans="2:20" ht="16.5">
+    <row r="22" spans="2:20" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B22" s="7"/>
       <c r="C22" s="7"/>
       <c r="D22" s="7"/>
@@ -4353,7 +4353,7 @@
       <c r="S22"/>
       <c r="T22"/>
     </row>
-    <row r="23" spans="2:20" ht="16.5">
+    <row r="23" spans="2:20" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B23" s="7"/>
       <c r="C23" s="7"/>
       <c r="D23" s="7"/>
@@ -4384,7 +4384,7 @@
       <c r="S23"/>
       <c r="T23"/>
     </row>
-    <row r="24" spans="2:20" ht="16.5">
+    <row r="24" spans="2:20" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B24" s="7"/>
       <c r="C24" s="7"/>
       <c r="D24" s="7"/>
@@ -4415,7 +4415,7 @@
       <c r="S24"/>
       <c r="T24"/>
     </row>
-    <row r="25" spans="2:20" ht="16.5">
+    <row r="25" spans="2:20" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B25" s="7"/>
       <c r="C25" s="7"/>
       <c r="D25" s="7"/>
@@ -4446,7 +4446,7 @@
       <c r="S25"/>
       <c r="T25"/>
     </row>
-    <row r="26" spans="2:20" ht="16.5">
+    <row r="26" spans="2:20" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B26" s="7"/>
       <c r="C26" s="7"/>
       <c r="D26" s="7"/>
@@ -4477,7 +4477,7 @@
       <c r="S26"/>
       <c r="T26"/>
     </row>
-    <row r="27" spans="2:20" ht="16.5">
+    <row r="27" spans="2:20" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B27" s="7">
         <v>155</v>
       </c>
@@ -4522,7 +4522,7 @@
       <c r="S27"/>
       <c r="T27"/>
     </row>
-    <row r="28" spans="2:20" ht="16.5">
+    <row r="28" spans="2:20" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B28" s="7"/>
       <c r="C28" s="5"/>
       <c r="D28" s="7"/>
@@ -4553,7 +4553,7 @@
       <c r="S28"/>
       <c r="T28"/>
     </row>
-    <row r="29" spans="2:20" ht="16.5">
+    <row r="29" spans="2:20" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B29" s="7"/>
       <c r="C29" s="5"/>
       <c r="D29" s="7"/>
@@ -4584,7 +4584,7 @@
       <c r="S29"/>
       <c r="T29"/>
     </row>
-    <row r="30" spans="2:20" ht="16.5">
+    <row r="30" spans="2:20" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B30" s="7"/>
       <c r="C30" s="5"/>
       <c r="D30" s="7"/>
@@ -4615,7 +4615,7 @@
       <c r="S30"/>
       <c r="T30"/>
     </row>
-    <row r="31" spans="2:20" ht="16.5">
+    <row r="31" spans="2:20" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B31" s="7"/>
       <c r="C31" s="5"/>
       <c r="D31" s="7"/>
@@ -4646,7 +4646,7 @@
       <c r="S31"/>
       <c r="T31"/>
     </row>
-    <row r="32" spans="2:20" ht="16.5">
+    <row r="32" spans="2:20" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B32" s="7"/>
       <c r="C32" s="5"/>
       <c r="D32" s="7"/>
@@ -4677,7 +4677,7 @@
       <c r="S32"/>
       <c r="T32"/>
     </row>
-    <row r="33" spans="2:20" ht="16.5">
+    <row r="33" spans="2:20" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B33" s="7"/>
       <c r="C33" s="5"/>
       <c r="D33" s="7"/>
@@ -4708,7 +4708,7 @@
       <c r="S33"/>
       <c r="T33"/>
     </row>
-    <row r="34" spans="2:20" ht="16.5">
+    <row r="34" spans="2:20" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B34" s="7"/>
       <c r="C34" s="5"/>
       <c r="D34" s="7"/>
@@ -4739,7 +4739,7 @@
       <c r="S34"/>
       <c r="T34"/>
     </row>
-    <row r="35" spans="2:20" ht="16.5">
+    <row r="35" spans="2:20" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B35" s="7"/>
       <c r="C35" s="5"/>
       <c r="D35" s="7"/>
@@ -4770,7 +4770,7 @@
       <c r="S35"/>
       <c r="T35"/>
     </row>
-    <row r="36" spans="2:20" ht="16.5">
+    <row r="36" spans="2:20" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B36" s="7"/>
       <c r="C36" s="5"/>
       <c r="D36" s="7"/>
@@ -4801,7 +4801,7 @@
       <c r="S36"/>
       <c r="T36"/>
     </row>
-    <row r="37" spans="2:20" ht="16.5">
+    <row r="37" spans="2:20" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B37" s="7">
         <v>374</v>
       </c>
@@ -4846,7 +4846,7 @@
       <c r="S37"/>
       <c r="T37"/>
     </row>
-    <row r="38" spans="2:20" ht="16.5">
+    <row r="38" spans="2:20" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B38" s="7"/>
       <c r="C38" s="5"/>
       <c r="D38" s="7"/>
@@ -4877,7 +4877,7 @@
       <c r="S38"/>
       <c r="T38"/>
     </row>
-    <row r="39" spans="2:20" ht="16.5">
+    <row r="39" spans="2:20" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B39" s="7"/>
       <c r="C39" s="5"/>
       <c r="D39" s="7"/>
@@ -4908,7 +4908,7 @@
       <c r="S39"/>
       <c r="T39"/>
     </row>
-    <row r="40" spans="2:20" ht="16.5">
+    <row r="40" spans="2:20" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B40" s="7"/>
       <c r="C40" s="5"/>
       <c r="D40" s="7"/>
@@ -4939,7 +4939,7 @@
       <c r="S40"/>
       <c r="T40"/>
     </row>
-    <row r="41" spans="2:20" ht="16.5">
+    <row r="41" spans="2:20" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B41" s="7"/>
       <c r="C41" s="5"/>
       <c r="D41" s="7"/>
@@ -4970,7 +4970,7 @@
       <c r="S41"/>
       <c r="T41"/>
     </row>
-    <row r="42" spans="2:20" ht="16.5">
+    <row r="42" spans="2:20" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B42" s="7"/>
       <c r="C42" s="5"/>
       <c r="D42" s="7"/>
@@ -5001,7 +5001,7 @@
       <c r="S42"/>
       <c r="T42"/>
     </row>
-    <row r="43" spans="2:20" ht="16.5">
+    <row r="43" spans="2:20" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B43" s="7"/>
       <c r="C43" s="5"/>
       <c r="D43" s="7"/>
@@ -5032,7 +5032,7 @@
       <c r="S43"/>
       <c r="T43"/>
     </row>
-    <row r="44" spans="2:20" ht="16.5">
+    <row r="44" spans="2:20" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B44" s="7">
         <v>376</v>
       </c>
@@ -5077,7 +5077,7 @@
       <c r="S44"/>
       <c r="T44"/>
     </row>
-    <row r="45" spans="2:20" ht="16.5">
+    <row r="45" spans="2:20" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B45" s="7"/>
       <c r="C45" s="5"/>
       <c r="D45" s="7"/>
@@ -5108,7 +5108,7 @@
       <c r="S45"/>
       <c r="T45"/>
     </row>
-    <row r="46" spans="2:20" ht="16.5">
+    <row r="46" spans="2:20" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B46" s="7"/>
       <c r="C46" s="7"/>
       <c r="D46" s="7"/>
@@ -5139,7 +5139,7 @@
       <c r="S46"/>
       <c r="T46"/>
     </row>
-    <row r="47" spans="2:20" ht="16.5">
+    <row r="47" spans="2:20" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B47" s="7"/>
       <c r="C47" s="7"/>
       <c r="D47" s="7"/>
@@ -5170,7 +5170,7 @@
       <c r="S47"/>
       <c r="T47"/>
     </row>
-    <row r="48" spans="2:20" ht="16.5">
+    <row r="48" spans="2:20" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B48" s="7"/>
       <c r="C48" s="7"/>
       <c r="D48" s="7"/>
@@ -5201,7 +5201,7 @@
       <c r="S48"/>
       <c r="T48"/>
     </row>
-    <row r="49" spans="2:20" ht="16.5">
+    <row r="49" spans="2:20" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B49" s="7"/>
       <c r="C49" s="7"/>
       <c r="D49" s="7"/>
@@ -5232,7 +5232,7 @@
       <c r="S49"/>
       <c r="T49"/>
     </row>
-    <row r="50" spans="2:20" ht="16.5">
+    <row r="50" spans="2:20" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B50" s="7"/>
       <c r="C50" s="7"/>
       <c r="D50" s="7"/>
@@ -5263,7 +5263,7 @@
       <c r="S50"/>
       <c r="T50"/>
     </row>
-    <row r="51" spans="2:20" ht="16.5">
+    <row r="51" spans="2:20" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B51" s="7">
         <v>375</v>
       </c>
@@ -5308,7 +5308,7 @@
       <c r="S51"/>
       <c r="T51"/>
     </row>
-    <row r="52" spans="2:20" ht="16.5">
+    <row r="52" spans="2:20" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B52" s="7"/>
       <c r="C52" s="7"/>
       <c r="D52" s="12"/>
@@ -5339,7 +5339,7 @@
       <c r="S52"/>
       <c r="T52"/>
     </row>
-    <row r="53" spans="2:20" ht="16.5">
+    <row r="53" spans="2:20" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B53" s="7"/>
       <c r="C53" s="7"/>
       <c r="D53" s="12"/>
@@ -5370,7 +5370,7 @@
       <c r="S53"/>
       <c r="T53"/>
     </row>
-    <row r="54" spans="2:20" ht="16.5">
+    <row r="54" spans="2:20" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B54" s="7"/>
       <c r="C54" s="7"/>
       <c r="D54" s="12"/>
@@ -5401,7 +5401,7 @@
       <c r="S54"/>
       <c r="T54"/>
     </row>
-    <row r="55" spans="2:20" ht="16.5">
+    <row r="55" spans="2:20" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B55" s="7"/>
       <c r="C55" s="7"/>
       <c r="D55" s="12"/>
@@ -5432,7 +5432,7 @@
       <c r="S55"/>
       <c r="T55"/>
     </row>
-    <row r="56" spans="2:20" ht="16.5">
+    <row r="56" spans="2:20" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B56" s="7"/>
       <c r="C56" s="7"/>
       <c r="D56" s="12"/>
@@ -5463,7 +5463,7 @@
       <c r="S56"/>
       <c r="T56"/>
     </row>
-    <row r="57" spans="2:20" ht="16.5">
+    <row r="57" spans="2:20" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B57" s="7"/>
       <c r="C57" s="7"/>
       <c r="D57" s="12"/>
@@ -5494,7 +5494,7 @@
       <c r="S57"/>
       <c r="T57"/>
     </row>
-    <row r="58" spans="2:20" ht="16.5">
+    <row r="58" spans="2:20" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B58" s="7">
         <v>30014</v>
       </c>
@@ -5533,7 +5533,7 @@
       <c r="S58"/>
       <c r="T58"/>
     </row>
-    <row r="59" spans="2:20" ht="16.5">
+    <row r="59" spans="2:20" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B59" s="7">
         <v>20010</v>
       </c>
@@ -5574,7 +5574,7 @@
       <c r="S59"/>
       <c r="T59"/>
     </row>
-    <row r="60" spans="2:20" ht="16.5">
+    <row r="60" spans="2:20" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B60" s="7"/>
       <c r="C60" s="7"/>
       <c r="D60" s="12"/>
@@ -5603,7 +5603,7 @@
       <c r="S60"/>
       <c r="T60"/>
     </row>
-    <row r="61" spans="2:20" ht="16.5">
+    <row r="61" spans="2:20" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B61" s="7"/>
       <c r="C61" s="7"/>
       <c r="D61" s="7"/>
@@ -5632,7 +5632,7 @@
       <c r="S61"/>
       <c r="T61"/>
     </row>
-    <row r="62" spans="2:20" ht="16.5">
+    <row r="62" spans="2:20" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B62" s="7"/>
       <c r="C62" s="7"/>
       <c r="D62" s="7"/>
@@ -5661,7 +5661,7 @@
       <c r="S62"/>
       <c r="T62"/>
     </row>
-    <row r="63" spans="2:20" ht="16.5">
+    <row r="63" spans="2:20" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B63" s="7"/>
       <c r="C63" s="7"/>
       <c r="D63" s="7"/>
@@ -5690,7 +5690,7 @@
       <c r="S63"/>
       <c r="T63"/>
     </row>
-    <row r="64" spans="2:20" ht="16.5">
+    <row r="64" spans="2:20" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B64" s="7"/>
       <c r="C64" s="7"/>
       <c r="D64" s="7"/>
@@ -5719,7 +5719,7 @@
       <c r="S64"/>
       <c r="T64"/>
     </row>
-    <row r="65" spans="2:20" ht="16.5">
+    <row r="65" spans="2:20" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B65" s="7"/>
       <c r="C65" s="7"/>
       <c r="D65" s="12"/>
@@ -5748,7 +5748,7 @@
       <c r="S65"/>
       <c r="T65"/>
     </row>
-    <row r="66" spans="2:20" ht="16.5">
+    <row r="66" spans="2:20" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B66" s="7"/>
       <c r="C66" s="7"/>
       <c r="D66" s="12"/>
@@ -5777,7 +5777,7 @@
       <c r="S66"/>
       <c r="T66"/>
     </row>
-    <row r="67" spans="2:20" ht="16.5">
+    <row r="67" spans="2:20" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B67" s="7">
         <v>1111</v>
       </c>
@@ -5818,7 +5818,7 @@
       <c r="S67"/>
       <c r="T67"/>
     </row>
-    <row r="68" spans="2:20" ht="16.5">
+    <row r="68" spans="2:20" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B68" s="7"/>
       <c r="C68" s="7"/>
       <c r="D68" s="12"/>
@@ -5843,7 +5843,7 @@
       <c r="S68"/>
       <c r="T68"/>
     </row>
-    <row r="69" spans="2:20" ht="16.5">
+    <row r="69" spans="2:20" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B69" s="7"/>
       <c r="C69" s="7"/>
       <c r="D69" s="12"/>
@@ -5868,7 +5868,7 @@
       <c r="S69"/>
       <c r="T69"/>
     </row>
-    <row r="70" spans="2:20" ht="16.5">
+    <row r="70" spans="2:20" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B70" s="7"/>
       <c r="C70" s="7"/>
       <c r="D70" s="12"/>
@@ -5893,7 +5893,7 @@
       <c r="S70"/>
       <c r="T70"/>
     </row>
-    <row r="71" spans="2:20" ht="16.5">
+    <row r="71" spans="2:20" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B71" s="7"/>
       <c r="C71" s="7"/>
       <c r="D71" s="12"/>
@@ -5918,7 +5918,7 @@
       <c r="S71"/>
       <c r="T71"/>
     </row>
-    <row r="72" spans="2:20" ht="16.5">
+    <row r="72" spans="2:20" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B72" s="7">
         <v>1112</v>
       </c>
@@ -5959,7 +5959,7 @@
       <c r="S72"/>
       <c r="T72"/>
     </row>
-    <row r="73" spans="2:20" ht="16.5">
+    <row r="73" spans="2:20" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B73" s="7"/>
       <c r="C73" s="7"/>
       <c r="D73" s="12"/>
@@ -5984,7 +5984,7 @@
       <c r="S73"/>
       <c r="T73"/>
     </row>
-    <row r="74" spans="2:20" ht="16.5">
+    <row r="74" spans="2:20" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B74" s="7"/>
       <c r="C74" s="7"/>
       <c r="D74" s="12"/>
@@ -6009,7 +6009,7 @@
       <c r="S74"/>
       <c r="T74"/>
     </row>
-    <row r="75" spans="2:20" ht="16.5">
+    <row r="75" spans="2:20" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B75" s="7"/>
       <c r="C75" s="7"/>
       <c r="D75" s="12"/>
@@ -6034,7 +6034,7 @@
       <c r="S75"/>
       <c r="T75"/>
     </row>
-    <row r="76" spans="2:20" ht="16.5">
+    <row r="76" spans="2:20" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B76" s="7"/>
       <c r="C76" s="7"/>
       <c r="D76" s="7"/>
@@ -6059,7 +6059,7 @@
       <c r="S76"/>
       <c r="T76"/>
     </row>
-    <row r="77" spans="2:20">
+    <row r="77" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B77" s="7">
         <v>421113</v>
       </c>
@@ -6098,7 +6098,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="78" spans="2:20">
+    <row r="78" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B78" s="7">
         <v>421114</v>
       </c>
@@ -6137,7 +6137,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="79" spans="2:20">
+    <row r="79" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B79" s="7"/>
       <c r="C79" s="7"/>
       <c r="D79" s="7"/>
@@ -6154,7 +6154,7 @@
       <c r="O79" s="7"/>
       <c r="P79" s="11"/>
     </row>
-    <row r="80" spans="2:20">
+    <row r="80" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B80" s="7"/>
       <c r="C80" s="7"/>
       <c r="D80" s="7"/>
@@ -6171,7 +6171,7 @@
       <c r="O80" s="7"/>
       <c r="P80" s="11"/>
     </row>
-    <row r="81" spans="2:16">
+    <row r="81" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B81" s="7"/>
       <c r="C81" s="7"/>
       <c r="D81" s="7"/>
@@ -6188,7 +6188,7 @@
       <c r="O81" s="7"/>
       <c r="P81" s="11"/>
     </row>
-    <row r="82" spans="2:16">
+    <row r="82" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B82" s="7"/>
       <c r="C82" s="7"/>
       <c r="D82" s="7"/>
@@ -6205,7 +6205,7 @@
       <c r="O82" s="7"/>
       <c r="P82" s="11"/>
     </row>
-    <row r="83" spans="2:16">
+    <row r="83" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B83" s="7"/>
       <c r="C83" s="7"/>
       <c r="D83" s="12"/>
@@ -6222,7 +6222,7 @@
       <c r="O83" s="7"/>
       <c r="P83" s="14"/>
     </row>
-    <row r="84" spans="2:16">
+    <row r="84" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B84" s="7"/>
       <c r="C84" s="7"/>
       <c r="D84" s="12"/>
@@ -6253,13 +6253,13 @@
   <dimension ref="A1:T58"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="F16" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="J41" sqref="J41"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="topRight"/>
+      <selection pane="bottomRight" activeCell="F55" sqref="F55"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="10.25" style="34" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.125" style="8" customWidth="1"/>
@@ -6280,7 +6280,7 @@
     <col min="21" max="16384" width="9" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A1" s="36" t="s">
         <v>0</v>
       </c>
@@ -6330,7 +6330,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:20" ht="16.5" customHeight="1">
+    <row r="2" spans="1:20" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="38">
         <v>45056</v>
       </c>
@@ -6370,7 +6370,7 @@
       <c r="O2" s="5"/>
       <c r="P2" s="5"/>
     </row>
-    <row r="3" spans="1:20">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A3" s="38">
         <v>45056</v>
       </c>
@@ -6396,7 +6396,7 @@
       <c r="O3" s="5"/>
       <c r="P3" s="5"/>
     </row>
-    <row r="4" spans="1:20">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A4" s="38">
         <v>45056</v>
       </c>
@@ -6422,7 +6422,7 @@
       <c r="O4" s="5"/>
       <c r="P4" s="5"/>
     </row>
-    <row r="5" spans="1:20">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A5" s="38">
         <v>45056</v>
       </c>
@@ -6448,7 +6448,7 @@
       <c r="O5" s="5"/>
       <c r="P5" s="5"/>
     </row>
-    <row r="6" spans="1:20">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A6" s="38">
         <v>45056</v>
       </c>
@@ -6474,7 +6474,7 @@
       <c r="O6" s="5"/>
       <c r="P6" s="5"/>
     </row>
-    <row r="7" spans="1:20">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A7" s="38">
         <v>45056</v>
       </c>
@@ -6500,7 +6500,7 @@
       <c r="O7" s="5"/>
       <c r="P7" s="5"/>
     </row>
-    <row r="8" spans="1:20">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A8" s="38">
         <v>45056</v>
       </c>
@@ -6526,7 +6526,7 @@
       <c r="O8" s="5"/>
       <c r="P8" s="5"/>
     </row>
-    <row r="9" spans="1:20">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A9" s="38">
         <v>45056</v>
       </c>
@@ -6552,7 +6552,7 @@
       <c r="O9" s="5"/>
       <c r="P9" s="5"/>
     </row>
-    <row r="10" spans="1:20">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A10" s="38">
         <v>45056</v>
       </c>
@@ -6578,7 +6578,7 @@
       <c r="O10" s="5"/>
       <c r="P10" s="5"/>
     </row>
-    <row r="11" spans="1:20">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A11" s="38">
         <v>45056</v>
       </c>
@@ -6604,7 +6604,7 @@
       <c r="O11" s="7"/>
       <c r="P11" s="7"/>
     </row>
-    <row r="12" spans="1:20" s="20" customFormat="1">
+    <row r="12" spans="1:20" s="20" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12" s="38">
         <v>45042</v>
       </c>
@@ -6650,7 +6650,7 @@
       <c r="S12" s="25"/>
       <c r="T12" s="25"/>
     </row>
-    <row r="13" spans="1:20" s="20" customFormat="1">
+    <row r="13" spans="1:20" s="20" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A13" s="38">
         <v>45042</v>
       </c>
@@ -6682,7 +6682,7 @@
       <c r="S13" s="25"/>
       <c r="T13" s="25"/>
     </row>
-    <row r="14" spans="1:20" s="20" customFormat="1">
+    <row r="14" spans="1:20" s="20" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A14" s="38">
         <v>45042</v>
       </c>
@@ -6714,7 +6714,7 @@
       <c r="S14" s="25"/>
       <c r="T14" s="25"/>
     </row>
-    <row r="15" spans="1:20" s="20" customFormat="1">
+    <row r="15" spans="1:20" s="20" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A15" s="38">
         <v>45042</v>
       </c>
@@ -6746,7 +6746,7 @@
       <c r="S15" s="25"/>
       <c r="T15" s="25"/>
     </row>
-    <row r="16" spans="1:20" s="20" customFormat="1">
+    <row r="16" spans="1:20" s="20" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A16" s="38">
         <v>45042</v>
       </c>
@@ -6778,7 +6778,7 @@
       <c r="S16" s="25"/>
       <c r="T16" s="25"/>
     </row>
-    <row r="17" spans="1:20" s="20" customFormat="1">
+    <row r="17" spans="1:20" s="20" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A17" s="38">
         <v>45042</v>
       </c>
@@ -6810,7 +6810,7 @@
       <c r="S17" s="25"/>
       <c r="T17" s="25"/>
     </row>
-    <row r="18" spans="1:20" s="20" customFormat="1">
+    <row r="18" spans="1:20" s="20" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A18" s="38">
         <v>45042</v>
       </c>
@@ -6842,7 +6842,7 @@
       <c r="S18" s="25"/>
       <c r="T18" s="25"/>
     </row>
-    <row r="19" spans="1:20" s="20" customFormat="1">
+    <row r="19" spans="1:20" s="20" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A19" s="38">
         <v>45042</v>
       </c>
@@ -6874,7 +6874,7 @@
       <c r="S19" s="25"/>
       <c r="T19" s="25"/>
     </row>
-    <row r="20" spans="1:20" s="20" customFormat="1">
+    <row r="20" spans="1:20" s="20" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A20" s="38">
         <v>45042</v>
       </c>
@@ -6906,7 +6906,7 @@
       <c r="S20" s="25"/>
       <c r="T20" s="25"/>
     </row>
-    <row r="21" spans="1:20" s="20" customFormat="1">
+    <row r="21" spans="1:20" s="20" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A21" s="38">
         <v>45042</v>
       </c>
@@ -6938,7 +6938,7 @@
       <c r="S21" s="25"/>
       <c r="T21" s="25"/>
     </row>
-    <row r="22" spans="1:20">
+    <row r="22" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A22" s="38">
         <v>45042</v>
       </c>
@@ -6982,7 +6982,7 @@
       <c r="O22" s="7"/>
       <c r="P22" s="7"/>
     </row>
-    <row r="23" spans="1:20">
+    <row r="23" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A23" s="38">
         <v>45042</v>
       </c>
@@ -7012,7 +7012,7 @@
       <c r="O23" s="7"/>
       <c r="P23" s="7"/>
     </row>
-    <row r="24" spans="1:20">
+    <row r="24" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A24" s="38">
         <v>45042</v>
       </c>
@@ -7042,7 +7042,7 @@
       <c r="O24" s="7"/>
       <c r="P24" s="7"/>
     </row>
-    <row r="25" spans="1:20">
+    <row r="25" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A25" s="38">
         <v>45042</v>
       </c>
@@ -7072,7 +7072,7 @@
       <c r="O25" s="7"/>
       <c r="P25" s="7"/>
     </row>
-    <row r="26" spans="1:20">
+    <row r="26" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A26" s="38">
         <v>45042</v>
       </c>
@@ -7102,7 +7102,7 @@
       <c r="O26" s="7"/>
       <c r="P26" s="7"/>
     </row>
-    <row r="27" spans="1:20">
+    <row r="27" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A27" s="38">
         <v>45042</v>
       </c>
@@ -7132,7 +7132,7 @@
       <c r="O27" s="7"/>
       <c r="P27" s="7"/>
     </row>
-    <row r="28" spans="1:20">
+    <row r="28" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A28" s="38">
         <v>45042</v>
       </c>
@@ -7162,7 +7162,7 @@
       <c r="O28" s="7"/>
       <c r="P28" s="7"/>
     </row>
-    <row r="29" spans="1:20" s="20" customFormat="1">
+    <row r="29" spans="1:20" s="20" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A29" s="38">
         <v>45042</v>
       </c>
@@ -7210,7 +7210,7 @@
       <c r="S29" s="25"/>
       <c r="T29" s="25"/>
     </row>
-    <row r="30" spans="1:20" s="20" customFormat="1">
+    <row r="30" spans="1:20" s="20" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A30" s="38">
         <v>45042</v>
       </c>
@@ -7244,7 +7244,7 @@
       <c r="S30" s="25"/>
       <c r="T30" s="25"/>
     </row>
-    <row r="31" spans="1:20" s="20" customFormat="1">
+    <row r="31" spans="1:20" s="20" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A31" s="38">
         <v>45042</v>
       </c>
@@ -7278,7 +7278,7 @@
       <c r="S31" s="25"/>
       <c r="T31" s="25"/>
     </row>
-    <row r="32" spans="1:20" s="20" customFormat="1">
+    <row r="32" spans="1:20" s="20" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A32" s="38">
         <v>45042</v>
       </c>
@@ -7312,7 +7312,7 @@
       <c r="S32" s="25"/>
       <c r="T32" s="25"/>
     </row>
-    <row r="33" spans="1:20" s="20" customFormat="1">
+    <row r="33" spans="1:20" s="20" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A33" s="38">
         <v>45042</v>
       </c>
@@ -7346,7 +7346,7 @@
       <c r="S33" s="25"/>
       <c r="T33" s="25"/>
     </row>
-    <row r="34" spans="1:20" s="20" customFormat="1">
+    <row r="34" spans="1:20" s="20" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A34" s="38">
         <v>45042</v>
       </c>
@@ -7380,7 +7380,7 @@
       <c r="S34" s="25"/>
       <c r="T34" s="25"/>
     </row>
-    <row r="35" spans="1:20" s="20" customFormat="1">
+    <row r="35" spans="1:20" s="20" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A35" s="38">
         <v>45042</v>
       </c>
@@ -7414,7 +7414,7 @@
       <c r="S35" s="25"/>
       <c r="T35" s="25"/>
     </row>
-    <row r="36" spans="1:20">
+    <row r="36" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A36" s="34">
         <v>45041</v>
       </c>
@@ -7452,7 +7452,7 @@
       <c r="O36" s="13"/>
       <c r="P36" s="13"/>
     </row>
-    <row r="37" spans="1:20" s="20" customFormat="1">
+    <row r="37" spans="1:20" s="20" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A37" s="37">
         <v>45041</v>
       </c>
@@ -7496,7 +7496,7 @@
       <c r="S37" s="25"/>
       <c r="T37" s="25"/>
     </row>
-    <row r="38" spans="1:20" s="20" customFormat="1">
+    <row r="38" spans="1:20" s="20" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A38" s="37">
         <v>45041</v>
       </c>
@@ -7528,7 +7528,7 @@
       <c r="S38" s="25"/>
       <c r="T38" s="25"/>
     </row>
-    <row r="39" spans="1:20" s="20" customFormat="1">
+    <row r="39" spans="1:20" s="20" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A39" s="37">
         <v>45041</v>
       </c>
@@ -7560,7 +7560,7 @@
       <c r="S39" s="25"/>
       <c r="T39" s="25"/>
     </row>
-    <row r="40" spans="1:20" s="20" customFormat="1">
+    <row r="40" spans="1:20" s="20" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A40" s="38">
         <v>45042</v>
       </c>
@@ -7592,7 +7592,7 @@
       <c r="S40" s="25"/>
       <c r="T40" s="25"/>
     </row>
-    <row r="41" spans="1:20" s="20" customFormat="1">
+    <row r="41" spans="1:20" s="20" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A41" s="37">
         <v>45041</v>
       </c>
@@ -7624,7 +7624,7 @@
       <c r="S41" s="25"/>
       <c r="T41" s="25"/>
     </row>
-    <row r="42" spans="1:20" s="20" customFormat="1">
+    <row r="42" spans="1:20" s="20" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A42" s="37">
         <v>45041</v>
       </c>
@@ -7655,7 +7655,7 @@
       <c r="S42" s="25"/>
       <c r="T42" s="25"/>
     </row>
-    <row r="43" spans="1:20" s="20" customFormat="1">
+    <row r="43" spans="1:20" s="20" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A43" s="37">
         <v>45041</v>
       </c>
@@ -7687,7 +7687,7 @@
       <c r="S43" s="25"/>
       <c r="T43" s="25"/>
     </row>
-    <row r="44" spans="1:20" s="20" customFormat="1">
+    <row r="44" spans="1:20" s="20" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A44" s="38">
         <v>45042</v>
       </c>
@@ -7719,7 +7719,7 @@
       <c r="S44" s="25"/>
       <c r="T44" s="25"/>
     </row>
-    <row r="45" spans="1:20" s="20" customFormat="1">
+    <row r="45" spans="1:20" s="20" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A45" s="38">
         <v>45042</v>
       </c>
@@ -7751,7 +7751,7 @@
       <c r="S45" s="25"/>
       <c r="T45" s="25"/>
     </row>
-    <row r="46" spans="1:20">
+    <row r="46" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A46" s="38">
         <v>45041</v>
       </c>
@@ -7789,7 +7789,7 @@
       <c r="O46" s="13"/>
       <c r="P46" s="13"/>
     </row>
-    <row r="47" spans="1:20">
+    <row r="47" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A47" s="34">
         <v>45041</v>
       </c>
@@ -7813,7 +7813,7 @@
       <c r="O47" s="13"/>
       <c r="P47" s="13"/>
     </row>
-    <row r="48" spans="1:20">
+    <row r="48" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A48" s="34">
         <v>45041</v>
       </c>
@@ -7837,7 +7837,7 @@
       <c r="O48" s="13"/>
       <c r="P48" s="13"/>
     </row>
-    <row r="49" spans="1:20">
+    <row r="49" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A49" s="34">
         <v>45041</v>
       </c>
@@ -7861,7 +7861,7 @@
       <c r="O49" s="13"/>
       <c r="P49" s="13"/>
     </row>
-    <row r="50" spans="1:20">
+    <row r="50" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A50" s="34">
         <v>45041</v>
       </c>
@@ -7885,7 +7885,7 @@
       <c r="O50" s="13"/>
       <c r="P50" s="13"/>
     </row>
-    <row r="51" spans="1:20">
+    <row r="51" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A51" s="34">
         <v>45041</v>
       </c>
@@ -7909,7 +7909,7 @@
       <c r="O51" s="13"/>
       <c r="P51" s="13"/>
     </row>
-    <row r="52" spans="1:20">
+    <row r="52" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A52" s="34">
         <v>45041</v>
       </c>
@@ -7933,7 +7933,7 @@
       <c r="O52" s="13"/>
       <c r="P52" s="13"/>
     </row>
-    <row r="53" spans="1:20" s="20" customFormat="1">
+    <row r="53" spans="1:20" s="20" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A53" s="38">
         <v>45041</v>
       </c>
@@ -7975,7 +7975,7 @@
       <c r="S53" s="25"/>
       <c r="T53" s="25"/>
     </row>
-    <row r="54" spans="1:20" s="20" customFormat="1">
+    <row r="54" spans="1:20" s="20" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A54" s="37">
         <v>45041</v>
       </c>
@@ -8003,7 +8003,7 @@
       <c r="S54" s="25"/>
       <c r="T54" s="25"/>
     </row>
-    <row r="55" spans="1:20" s="20" customFormat="1">
+    <row r="55" spans="1:20" s="20" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A55" s="37">
         <v>45041</v>
       </c>
@@ -8031,7 +8031,7 @@
       <c r="S55" s="25"/>
       <c r="T55" s="25"/>
     </row>
-    <row r="56" spans="1:20" s="20" customFormat="1">
+    <row r="56" spans="1:20" s="20" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A56" s="37">
         <v>45041</v>
       </c>
@@ -8059,7 +8059,7 @@
       <c r="S56" s="25"/>
       <c r="T56" s="25"/>
     </row>
-    <row r="57" spans="1:20" s="20" customFormat="1">
+    <row r="57" spans="1:20" s="20" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A57" s="37">
         <v>45041</v>
       </c>
@@ -8087,7 +8087,7 @@
       <c r="S57" s="25"/>
       <c r="T57" s="25"/>
     </row>
-    <row r="58" spans="1:20" s="20" customFormat="1">
+    <row r="58" spans="1:20" s="20" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A58" s="37">
         <v>45041</v>
       </c>
@@ -8123,7 +8123,7 @@
       <selection pane="bottomRight" activeCell="L4" sqref="L4"/>
       <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
       <pageSetup paperSize="9" orientation="portrait" verticalDpi="0"/>
-      <autoFilter ref="B1:T58" xr:uid="{FF35DCE1-E53C-4DE1-857D-A7444BA7BD5D}"/>
+      <autoFilter ref="B1:T58" xr:uid="{7B984E71-0C7C-47E3-B5F5-70095F3C3A8D}"/>
     </customSheetView>
   </customSheetViews>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -8139,12 +8139,12 @@
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B28" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight"/>
+      <selection pane="bottomLeft"/>
       <selection pane="bottomRight" activeCell="I57" sqref="I57"/>
-      <selection pane="bottomLeft"/>
-      <selection pane="topRight"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="9" style="8"/>
     <col min="2" max="2" width="11.125" style="8" customWidth="1"/>
@@ -8164,7 +8164,7 @@
     <col min="20" max="16384" width="9" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -8211,7 +8211,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:19" ht="16.5" customHeight="1">
+    <row r="2" spans="1:19" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B2" s="5">
         <v>150</v>
       </c>
@@ -8247,7 +8247,7 @@
       <c r="N2" s="5"/>
       <c r="O2" s="5"/>
     </row>
-    <row r="3" spans="1:19">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B3" s="5"/>
       <c r="C3" s="5"/>
       <c r="D3" s="5"/>
@@ -8269,7 +8269,7 @@
       <c r="N3" s="5"/>
       <c r="O3" s="5"/>
     </row>
-    <row r="4" spans="1:19">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B4" s="5"/>
       <c r="C4" s="5"/>
       <c r="D4" s="5"/>
@@ -8291,7 +8291,7 @@
       <c r="N4" s="5"/>
       <c r="O4" s="5"/>
     </row>
-    <row r="5" spans="1:19">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B5" s="5"/>
       <c r="C5" s="5"/>
       <c r="D5" s="5"/>
@@ -8313,7 +8313,7 @@
       <c r="N5" s="5"/>
       <c r="O5" s="5"/>
     </row>
-    <row r="6" spans="1:19">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
@@ -8335,7 +8335,7 @@
       <c r="N6" s="5"/>
       <c r="O6" s="5"/>
     </row>
-    <row r="7" spans="1:19">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>
       <c r="D7" s="5"/>
@@ -8357,7 +8357,7 @@
       <c r="N7" s="5"/>
       <c r="O7" s="5"/>
     </row>
-    <row r="8" spans="1:19">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B8" s="5"/>
       <c r="C8" s="5"/>
       <c r="D8" s="5"/>
@@ -8379,7 +8379,7 @@
       <c r="N8" s="5"/>
       <c r="O8" s="5"/>
     </row>
-    <row r="9" spans="1:19">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B9" s="5"/>
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
@@ -8401,7 +8401,7 @@
       <c r="N9" s="5"/>
       <c r="O9" s="5"/>
     </row>
-    <row r="10" spans="1:19">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B10" s="5"/>
       <c r="C10" s="5"/>
       <c r="D10" s="5"/>
@@ -8423,7 +8423,7 @@
       <c r="N10" s="5"/>
       <c r="O10" s="5"/>
     </row>
-    <row r="11" spans="1:19">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B11" s="7"/>
       <c r="C11" s="7"/>
       <c r="D11" s="7"/>
@@ -8445,7 +8445,7 @@
       <c r="N11" s="7"/>
       <c r="O11" s="7"/>
     </row>
-    <row r="12" spans="1:19" s="20" customFormat="1">
+    <row r="12" spans="1:19" s="20" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B12" s="21">
         <v>151</v>
       </c>
@@ -8485,7 +8485,7 @@
       <c r="R12" s="25"/>
       <c r="S12" s="25"/>
     </row>
-    <row r="13" spans="1:19" s="20" customFormat="1">
+    <row r="13" spans="1:19" s="20" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B13" s="21"/>
       <c r="C13" s="22"/>
       <c r="D13" s="21"/>
@@ -8511,7 +8511,7 @@
       <c r="R13" s="25"/>
       <c r="S13" s="25"/>
     </row>
-    <row r="14" spans="1:19" s="20" customFormat="1">
+    <row r="14" spans="1:19" s="20" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B14" s="21"/>
       <c r="C14" s="22"/>
       <c r="D14" s="21"/>
@@ -8537,7 +8537,7 @@
       <c r="R14" s="25"/>
       <c r="S14" s="25"/>
     </row>
-    <row r="15" spans="1:19" s="20" customFormat="1">
+    <row r="15" spans="1:19" s="20" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B15" s="21"/>
       <c r="C15" s="22"/>
       <c r="D15" s="21"/>
@@ -8563,7 +8563,7 @@
       <c r="R15" s="25"/>
       <c r="S15" s="25"/>
     </row>
-    <row r="16" spans="1:19" s="20" customFormat="1">
+    <row r="16" spans="1:19" s="20" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B16" s="21"/>
       <c r="C16" s="22"/>
       <c r="D16" s="21"/>
@@ -8589,7 +8589,7 @@
       <c r="R16" s="25"/>
       <c r="S16" s="25"/>
     </row>
-    <row r="17" spans="2:19" s="20" customFormat="1">
+    <row r="17" spans="2:19" s="20" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B17" s="21"/>
       <c r="C17" s="22"/>
       <c r="D17" s="21"/>
@@ -8615,7 +8615,7 @@
       <c r="R17" s="25"/>
       <c r="S17" s="25"/>
     </row>
-    <row r="18" spans="2:19" s="20" customFormat="1">
+    <row r="18" spans="2:19" s="20" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B18" s="21"/>
       <c r="C18" s="22"/>
       <c r="D18" s="21"/>
@@ -8641,7 +8641,7 @@
       <c r="R18" s="25"/>
       <c r="S18" s="25"/>
     </row>
-    <row r="19" spans="2:19" s="20" customFormat="1">
+    <row r="19" spans="2:19" s="20" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B19" s="21"/>
       <c r="C19" s="22"/>
       <c r="D19" s="21"/>
@@ -8667,7 +8667,7 @@
       <c r="R19" s="25"/>
       <c r="S19" s="25"/>
     </row>
-    <row r="20" spans="2:19" s="20" customFormat="1">
+    <row r="20" spans="2:19" s="20" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B20" s="21"/>
       <c r="C20" s="22"/>
       <c r="D20" s="21"/>
@@ -8693,7 +8693,7 @@
       <c r="R20" s="25"/>
       <c r="S20" s="25"/>
     </row>
-    <row r="21" spans="2:19" s="20" customFormat="1">
+    <row r="21" spans="2:19" s="20" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B21" s="21"/>
       <c r="C21" s="22"/>
       <c r="D21" s="21"/>
@@ -8719,7 +8719,7 @@
       <c r="R21" s="25"/>
       <c r="S21" s="25"/>
     </row>
-    <row r="22" spans="2:19">
+    <row r="22" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B22" s="7">
         <v>370</v>
       </c>
@@ -8757,7 +8757,7 @@
       <c r="N22" s="7"/>
       <c r="O22" s="7"/>
     </row>
-    <row r="23" spans="2:19">
+    <row r="23" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B23" s="7"/>
       <c r="C23" s="5"/>
       <c r="D23" s="7"/>
@@ -8781,7 +8781,7 @@
       <c r="N23" s="7"/>
       <c r="O23" s="7"/>
     </row>
-    <row r="24" spans="2:19">
+    <row r="24" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B24" s="7"/>
       <c r="C24" s="5"/>
       <c r="D24" s="7"/>
@@ -8805,7 +8805,7 @@
       <c r="N24" s="7"/>
       <c r="O24" s="7"/>
     </row>
-    <row r="25" spans="2:19">
+    <row r="25" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B25" s="7"/>
       <c r="C25" s="5"/>
       <c r="D25" s="7"/>
@@ -8829,7 +8829,7 @@
       <c r="N25" s="7"/>
       <c r="O25" s="7"/>
     </row>
-    <row r="26" spans="2:19">
+    <row r="26" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B26" s="7"/>
       <c r="C26" s="5"/>
       <c r="D26" s="7"/>
@@ -8853,7 +8853,7 @@
       <c r="N26" s="7"/>
       <c r="O26" s="7"/>
     </row>
-    <row r="27" spans="2:19">
+    <row r="27" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B27" s="7"/>
       <c r="C27" s="5"/>
       <c r="D27" s="7"/>
@@ -8877,7 +8877,7 @@
       <c r="N27" s="7"/>
       <c r="O27" s="7"/>
     </row>
-    <row r="28" spans="2:19">
+    <row r="28" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B28" s="7"/>
       <c r="C28" s="5"/>
       <c r="D28" s="7"/>
@@ -8901,7 +8901,7 @@
       <c r="N28" s="7"/>
       <c r="O28" s="7"/>
     </row>
-    <row r="29" spans="2:19" s="20" customFormat="1">
+    <row r="29" spans="2:19" s="20" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B29" s="21">
         <v>371</v>
       </c>
@@ -8943,7 +8943,7 @@
       <c r="R29" s="25"/>
       <c r="S29" s="25"/>
     </row>
-    <row r="30" spans="2:19" s="20" customFormat="1">
+    <row r="30" spans="2:19" s="20" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B30" s="21"/>
       <c r="C30" s="22"/>
       <c r="D30" s="21"/>
@@ -8971,7 +8971,7 @@
       <c r="R30" s="25"/>
       <c r="S30" s="25"/>
     </row>
-    <row r="31" spans="2:19" s="20" customFormat="1">
+    <row r="31" spans="2:19" s="20" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B31" s="21"/>
       <c r="C31" s="21"/>
       <c r="D31" s="21"/>
@@ -8999,7 +8999,7 @@
       <c r="R31" s="25"/>
       <c r="S31" s="25"/>
     </row>
-    <row r="32" spans="2:19" s="20" customFormat="1">
+    <row r="32" spans="2:19" s="20" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B32" s="21"/>
       <c r="C32" s="21"/>
       <c r="D32" s="21"/>
@@ -9027,7 +9027,7 @@
       <c r="R32" s="25"/>
       <c r="S32" s="25"/>
     </row>
-    <row r="33" spans="2:19" s="20" customFormat="1">
+    <row r="33" spans="2:19" s="20" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B33" s="21"/>
       <c r="C33" s="21"/>
       <c r="D33" s="21"/>
@@ -9055,7 +9055,7 @@
       <c r="R33" s="25"/>
       <c r="S33" s="25"/>
     </row>
-    <row r="34" spans="2:19" s="20" customFormat="1">
+    <row r="34" spans="2:19" s="20" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B34" s="21"/>
       <c r="C34" s="21"/>
       <c r="D34" s="21"/>
@@ -9083,7 +9083,7 @@
       <c r="R34" s="25"/>
       <c r="S34" s="25"/>
     </row>
-    <row r="35" spans="2:19" s="20" customFormat="1">
+    <row r="35" spans="2:19" s="20" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B35" s="21"/>
       <c r="C35" s="21"/>
       <c r="D35" s="21"/>
@@ -9111,7 +9111,7 @@
       <c r="R35" s="25"/>
       <c r="S35" s="25"/>
     </row>
-    <row r="36" spans="2:19">
+    <row r="36" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B36" s="7">
         <v>30012</v>
       </c>
@@ -9145,7 +9145,7 @@
       <c r="N36" s="13"/>
       <c r="O36" s="13"/>
     </row>
-    <row r="37" spans="2:19" s="20" customFormat="1">
+    <row r="37" spans="2:19" s="20" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B37" s="21">
         <v>20008</v>
       </c>
@@ -9185,7 +9185,7 @@
       <c r="R37" s="25"/>
       <c r="S37" s="25"/>
     </row>
-    <row r="38" spans="2:19" s="20" customFormat="1">
+    <row r="38" spans="2:19" s="20" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B38" s="21"/>
       <c r="C38" s="21"/>
       <c r="D38" s="26"/>
@@ -9213,7 +9213,7 @@
       <c r="R38" s="25"/>
       <c r="S38" s="25"/>
     </row>
-    <row r="39" spans="2:19" s="20" customFormat="1">
+    <row r="39" spans="2:19" s="20" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B39" s="21"/>
       <c r="C39" s="21"/>
       <c r="D39" s="21"/>
@@ -9241,7 +9241,7 @@
       <c r="R39" s="25"/>
       <c r="S39" s="25"/>
     </row>
-    <row r="40" spans="2:19" s="20" customFormat="1">
+    <row r="40" spans="2:19" s="20" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B40" s="21"/>
       <c r="C40" s="21"/>
       <c r="D40" s="21"/>
@@ -9269,7 +9269,7 @@
       <c r="R40" s="25"/>
       <c r="S40" s="25"/>
     </row>
-    <row r="41" spans="2:19" s="20" customFormat="1">
+    <row r="41" spans="2:19" s="20" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B41" s="21"/>
       <c r="C41" s="21"/>
       <c r="D41" s="21"/>
@@ -9297,7 +9297,7 @@
       <c r="R41" s="25"/>
       <c r="S41" s="25"/>
     </row>
-    <row r="42" spans="2:19" s="20" customFormat="1">
+    <row r="42" spans="2:19" s="20" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B42" s="21"/>
       <c r="C42" s="21"/>
       <c r="D42" s="21"/>
@@ -9325,7 +9325,7 @@
       <c r="R42" s="25"/>
       <c r="S42" s="25"/>
     </row>
-    <row r="43" spans="2:19" s="20" customFormat="1">
+    <row r="43" spans="2:19" s="20" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B43" s="21"/>
       <c r="C43" s="21"/>
       <c r="D43" s="26"/>
@@ -9353,7 +9353,7 @@
       <c r="R43" s="25"/>
       <c r="S43" s="25"/>
     </row>
-    <row r="44" spans="2:19" s="20" customFormat="1">
+    <row r="44" spans="2:19" s="20" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B44" s="21"/>
       <c r="C44" s="21"/>
       <c r="D44" s="26"/>
@@ -9381,7 +9381,7 @@
       <c r="R44" s="25"/>
       <c r="S44" s="25"/>
     </row>
-    <row r="45" spans="2:19">
+    <row r="45" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B45" s="7">
         <v>1104</v>
       </c>
@@ -9415,7 +9415,7 @@
       <c r="N45" s="13"/>
       <c r="O45" s="13"/>
     </row>
-    <row r="46" spans="2:19">
+    <row r="46" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B46" s="7"/>
       <c r="C46" s="7"/>
       <c r="D46" s="12"/>
@@ -9435,7 +9435,7 @@
       <c r="N46" s="13"/>
       <c r="O46" s="13"/>
     </row>
-    <row r="47" spans="2:19">
+    <row r="47" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B47" s="7"/>
       <c r="C47" s="7"/>
       <c r="D47" s="12"/>
@@ -9455,7 +9455,7 @@
       <c r="N47" s="13"/>
       <c r="O47" s="13"/>
     </row>
-    <row r="48" spans="2:19">
+    <row r="48" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B48" s="7"/>
       <c r="C48" s="7"/>
       <c r="D48" s="12"/>
@@ -9475,7 +9475,7 @@
       <c r="N48" s="13"/>
       <c r="O48" s="13"/>
     </row>
-    <row r="49" spans="2:19">
+    <row r="49" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B49" s="7"/>
       <c r="C49" s="7"/>
       <c r="D49" s="12"/>
@@ -9495,7 +9495,7 @@
       <c r="N49" s="13"/>
       <c r="O49" s="13"/>
     </row>
-    <row r="50" spans="2:19">
+    <row r="50" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B50" s="7"/>
       <c r="C50" s="7"/>
       <c r="D50" s="12"/>
@@ -9515,7 +9515,7 @@
       <c r="N50" s="13"/>
       <c r="O50" s="13"/>
     </row>
-    <row r="51" spans="2:19" s="20" customFormat="1">
+    <row r="51" spans="2:19" s="20" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B51" s="21">
         <v>1105</v>
       </c>
@@ -9553,7 +9553,7 @@
       <c r="R51" s="25"/>
       <c r="S51" s="25"/>
     </row>
-    <row r="52" spans="2:19" s="20" customFormat="1">
+    <row r="52" spans="2:19" s="20" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B52" s="21"/>
       <c r="C52" s="21"/>
       <c r="D52" s="26"/>
@@ -9577,7 +9577,7 @@
       <c r="R52" s="25"/>
       <c r="S52" s="25"/>
     </row>
-    <row r="53" spans="2:19" s="20" customFormat="1">
+    <row r="53" spans="2:19" s="20" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B53" s="21"/>
       <c r="C53" s="21"/>
       <c r="D53" s="26"/>
@@ -9601,7 +9601,7 @@
       <c r="R53" s="25"/>
       <c r="S53" s="25"/>
     </row>
-    <row r="54" spans="2:19" s="20" customFormat="1">
+    <row r="54" spans="2:19" s="20" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B54" s="21"/>
       <c r="C54" s="21"/>
       <c r="D54" s="26"/>
@@ -9625,7 +9625,7 @@
       <c r="R54" s="25"/>
       <c r="S54" s="25"/>
     </row>
-    <row r="55" spans="2:19" s="20" customFormat="1">
+    <row r="55" spans="2:19" s="20" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B55" s="21"/>
       <c r="C55" s="21"/>
       <c r="D55" s="21"/>
@@ -9649,7 +9649,7 @@
       <c r="R55" s="25"/>
       <c r="S55" s="25"/>
     </row>
-    <row r="56" spans="2:19" s="20" customFormat="1">
+    <row r="56" spans="2:19" s="20" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B56" s="21"/>
       <c r="C56" s="21"/>
       <c r="D56" s="21"/>
@@ -9681,7 +9681,7 @@
       <selection pane="bottomRight" activeCell="A11" sqref="A11"/>
       <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
       <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
-      <autoFilter ref="B1:S56" xr:uid="{1A19EF48-E64E-4753-9F5B-3AB464489CF7}"/>
+      <autoFilter ref="B1:S56" xr:uid="{68EA2D54-2556-437B-8A7E-8B76E941F913}"/>
     </customSheetView>
   </customSheetViews>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -9700,7 +9700,7 @@
       <selection pane="bottomLeft" activeCell="J115" sqref="J115"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="9" style="8"/>
     <col min="2" max="2" width="7.5" style="8" bestFit="1" customWidth="1"/>
@@ -9718,7 +9718,7 @@
     <col min="18" max="16384" width="9" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -9769,7 +9769,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="16.5" customHeight="1">
+    <row r="2" spans="1:17" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B2" s="5">
         <v>146</v>
       </c>
@@ -9805,7 +9805,7 @@
         <v>44994</v>
       </c>
     </row>
-    <row r="3" spans="1:17">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B3" s="5"/>
       <c r="C3" s="5"/>
       <c r="D3" s="5"/>
@@ -9827,7 +9827,7 @@
       <c r="P3" s="9"/>
       <c r="Q3" s="9"/>
     </row>
-    <row r="4" spans="1:17">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B4" s="5"/>
       <c r="C4" s="5"/>
       <c r="D4" s="5"/>
@@ -9849,7 +9849,7 @@
       <c r="P4" s="9"/>
       <c r="Q4" s="9"/>
     </row>
-    <row r="5" spans="1:17">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B5" s="5"/>
       <c r="C5" s="5"/>
       <c r="D5" s="5"/>
@@ -9871,7 +9871,7 @@
       <c r="P5" s="9"/>
       <c r="Q5" s="9"/>
     </row>
-    <row r="6" spans="1:17">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
@@ -9893,7 +9893,7 @@
       <c r="P6" s="9"/>
       <c r="Q6" s="9"/>
     </row>
-    <row r="7" spans="1:17">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>
       <c r="D7" s="5"/>
@@ -9915,7 +9915,7 @@
       <c r="P7" s="9"/>
       <c r="Q7" s="9"/>
     </row>
-    <row r="8" spans="1:17">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B8" s="5"/>
       <c r="C8" s="5"/>
       <c r="D8" s="5"/>
@@ -9937,7 +9937,7 @@
       <c r="P8" s="9"/>
       <c r="Q8" s="9"/>
     </row>
-    <row r="9" spans="1:17">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B9" s="5"/>
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
@@ -9959,7 +9959,7 @@
       <c r="P9" s="9"/>
       <c r="Q9" s="9"/>
     </row>
-    <row r="10" spans="1:17">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B10" s="5"/>
       <c r="C10" s="5"/>
       <c r="D10" s="5"/>
@@ -9981,7 +9981,7 @@
       <c r="P10" s="9"/>
       <c r="Q10" s="9"/>
     </row>
-    <row r="11" spans="1:17">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B11" s="7"/>
       <c r="C11" s="7"/>
       <c r="D11" s="7"/>
@@ -10003,7 +10003,7 @@
       <c r="P11" s="7"/>
       <c r="Q11" s="7"/>
     </row>
-    <row r="12" spans="1:17">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B12" s="7">
         <v>147</v>
       </c>
@@ -10039,7 +10039,7 @@
         <v>45015</v>
       </c>
     </row>
-    <row r="13" spans="1:17">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B13" s="7"/>
       <c r="C13" s="7"/>
       <c r="D13" s="7"/>
@@ -10061,7 +10061,7 @@
       <c r="P13" s="7"/>
       <c r="Q13" s="7"/>
     </row>
-    <row r="14" spans="1:17">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B14" s="7"/>
       <c r="C14" s="7"/>
       <c r="D14" s="7"/>
@@ -10083,7 +10083,7 @@
       <c r="P14" s="7"/>
       <c r="Q14" s="7"/>
     </row>
-    <row r="15" spans="1:17">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B15" s="7"/>
       <c r="C15" s="7"/>
       <c r="D15" s="7"/>
@@ -10105,7 +10105,7 @@
       <c r="P15" s="7"/>
       <c r="Q15" s="7"/>
     </row>
-    <row r="16" spans="1:17">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B16" s="7"/>
       <c r="C16" s="7"/>
       <c r="D16" s="7"/>
@@ -10127,7 +10127,7 @@
       <c r="P16" s="7"/>
       <c r="Q16" s="7"/>
     </row>
-    <row r="17" spans="2:17">
+    <row r="17" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B17" s="7"/>
       <c r="C17" s="7"/>
       <c r="D17" s="7"/>
@@ -10149,7 +10149,7 @@
       <c r="P17" s="7"/>
       <c r="Q17" s="7"/>
     </row>
-    <row r="18" spans="2:17">
+    <row r="18" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B18" s="7"/>
       <c r="C18" s="7"/>
       <c r="D18" s="7"/>
@@ -10171,7 +10171,7 @@
       <c r="P18" s="7"/>
       <c r="Q18" s="7"/>
     </row>
-    <row r="19" spans="2:17">
+    <row r="19" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B19" s="7"/>
       <c r="C19" s="7"/>
       <c r="D19" s="7"/>
@@ -10193,7 +10193,7 @@
       <c r="P19" s="7"/>
       <c r="Q19" s="7"/>
     </row>
-    <row r="20" spans="2:17">
+    <row r="20" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B20" s="7"/>
       <c r="C20" s="7"/>
       <c r="D20" s="7"/>
@@ -10215,7 +10215,7 @@
       <c r="P20" s="7"/>
       <c r="Q20" s="7"/>
     </row>
-    <row r="21" spans="2:17">
+    <row r="21" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B21" s="7"/>
       <c r="C21" s="7"/>
       <c r="D21" s="7"/>
@@ -10237,7 +10237,7 @@
       <c r="P21" s="7"/>
       <c r="Q21" s="7"/>
     </row>
-    <row r="22" spans="2:17">
+    <row r="22" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B22" s="7">
         <v>148</v>
       </c>
@@ -10273,7 +10273,7 @@
         <v>45022</v>
       </c>
     </row>
-    <row r="23" spans="2:17">
+    <row r="23" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B23" s="7"/>
       <c r="C23" s="7"/>
       <c r="D23" s="7"/>
@@ -10295,7 +10295,7 @@
       <c r="P23" s="7"/>
       <c r="Q23" s="7"/>
     </row>
-    <row r="24" spans="2:17">
+    <row r="24" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B24" s="7"/>
       <c r="C24" s="7"/>
       <c r="D24" s="7"/>
@@ -10317,7 +10317,7 @@
       <c r="P24" s="7"/>
       <c r="Q24" s="7"/>
     </row>
-    <row r="25" spans="2:17">
+    <row r="25" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B25" s="7"/>
       <c r="C25" s="7"/>
       <c r="D25" s="7"/>
@@ -10339,7 +10339,7 @@
       <c r="P25" s="7"/>
       <c r="Q25" s="7"/>
     </row>
-    <row r="26" spans="2:17">
+    <row r="26" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B26" s="7"/>
       <c r="C26" s="7"/>
       <c r="D26" s="7"/>
@@ -10361,7 +10361,7 @@
       <c r="P26" s="7"/>
       <c r="Q26" s="7"/>
     </row>
-    <row r="27" spans="2:17">
+    <row r="27" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B27" s="7"/>
       <c r="C27" s="7"/>
       <c r="D27" s="7"/>
@@ -10383,7 +10383,7 @@
       <c r="P27" s="7"/>
       <c r="Q27" s="7"/>
     </row>
-    <row r="28" spans="2:17">
+    <row r="28" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B28" s="7"/>
       <c r="C28" s="7"/>
       <c r="D28" s="7"/>
@@ -10405,7 +10405,7 @@
       <c r="P28" s="7"/>
       <c r="Q28" s="7"/>
     </row>
-    <row r="29" spans="2:17">
+    <row r="29" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B29" s="7"/>
       <c r="C29" s="7"/>
       <c r="D29" s="7"/>
@@ -10427,7 +10427,7 @@
       <c r="P29" s="7"/>
       <c r="Q29" s="7"/>
     </row>
-    <row r="30" spans="2:17">
+    <row r="30" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B30" s="7"/>
       <c r="C30" s="7"/>
       <c r="D30" s="7"/>
@@ -10449,7 +10449,7 @@
       <c r="P30" s="7"/>
       <c r="Q30" s="7"/>
     </row>
-    <row r="31" spans="2:17">
+    <row r="31" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B31" s="7"/>
       <c r="C31" s="7"/>
       <c r="D31" s="7"/>
@@ -10471,7 +10471,7 @@
       <c r="P31" s="7"/>
       <c r="Q31" s="7"/>
     </row>
-    <row r="32" spans="2:17">
+    <row r="32" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B32" s="7"/>
       <c r="C32" s="7"/>
       <c r="D32" s="7"/>
@@ -10493,7 +10493,7 @@
       <c r="P32" s="7"/>
       <c r="Q32" s="7"/>
     </row>
-    <row r="33" spans="2:17">
+    <row r="33" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B33" s="7"/>
       <c r="C33" s="7"/>
       <c r="D33" s="7"/>
@@ -10515,7 +10515,7 @@
       <c r="P33" s="7"/>
       <c r="Q33" s="7"/>
     </row>
-    <row r="34" spans="2:17">
+    <row r="34" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B34" s="7"/>
       <c r="C34" s="7"/>
       <c r="D34" s="7"/>
@@ -10537,7 +10537,7 @@
       <c r="P34" s="7"/>
       <c r="Q34" s="7"/>
     </row>
-    <row r="35" spans="2:17">
+    <row r="35" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B35" s="7"/>
       <c r="C35" s="7"/>
       <c r="D35" s="7"/>
@@ -10559,7 +10559,7 @@
       <c r="P35" s="7"/>
       <c r="Q35" s="7"/>
     </row>
-    <row r="36" spans="2:17">
+    <row r="36" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B36" s="7"/>
       <c r="C36" s="7"/>
       <c r="D36" s="7"/>
@@ -10581,7 +10581,7 @@
       <c r="P36" s="7"/>
       <c r="Q36" s="7"/>
     </row>
-    <row r="37" spans="2:17">
+    <row r="37" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B37" s="7"/>
       <c r="C37" s="7"/>
       <c r="D37" s="7"/>
@@ -10603,7 +10603,7 @@
       <c r="P37" s="7"/>
       <c r="Q37" s="7"/>
     </row>
-    <row r="38" spans="2:17">
+    <row r="38" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B38" s="7"/>
       <c r="C38" s="7"/>
       <c r="D38" s="7"/>
@@ -10625,7 +10625,7 @@
       <c r="P38" s="7"/>
       <c r="Q38" s="7"/>
     </row>
-    <row r="39" spans="2:17">
+    <row r="39" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B39" s="7"/>
       <c r="C39" s="7"/>
       <c r="D39" s="7"/>
@@ -10647,7 +10647,7 @@
       <c r="P39" s="7"/>
       <c r="Q39" s="7"/>
     </row>
-    <row r="40" spans="2:17">
+    <row r="40" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B40" s="7"/>
       <c r="C40" s="7"/>
       <c r="D40" s="7"/>
@@ -10669,7 +10669,7 @@
       <c r="P40" s="7"/>
       <c r="Q40" s="7"/>
     </row>
-    <row r="41" spans="2:17">
+    <row r="41" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B41" s="7"/>
       <c r="C41" s="7"/>
       <c r="D41" s="7"/>
@@ -10691,7 +10691,7 @@
       <c r="P41" s="7"/>
       <c r="Q41" s="7"/>
     </row>
-    <row r="42" spans="2:17">
+    <row r="42" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B42" s="7">
         <v>149</v>
       </c>
@@ -10727,7 +10727,7 @@
         <v>45022</v>
       </c>
     </row>
-    <row r="43" spans="2:17">
+    <row r="43" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B43" s="7"/>
       <c r="C43" s="7"/>
       <c r="D43" s="7"/>
@@ -10749,7 +10749,7 @@
       <c r="P43" s="7"/>
       <c r="Q43" s="7"/>
     </row>
-    <row r="44" spans="2:17">
+    <row r="44" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B44" s="7"/>
       <c r="C44" s="7"/>
       <c r="D44" s="7"/>
@@ -10771,7 +10771,7 @@
       <c r="P44" s="7"/>
       <c r="Q44" s="7"/>
     </row>
-    <row r="45" spans="2:17">
+    <row r="45" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B45" s="7"/>
       <c r="C45" s="7"/>
       <c r="D45" s="7"/>
@@ -10793,7 +10793,7 @@
       <c r="P45" s="7"/>
       <c r="Q45" s="7"/>
     </row>
-    <row r="46" spans="2:17">
+    <row r="46" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B46" s="7"/>
       <c r="C46" s="7"/>
       <c r="D46" s="7"/>
@@ -10815,7 +10815,7 @@
       <c r="P46" s="7"/>
       <c r="Q46" s="7"/>
     </row>
-    <row r="47" spans="2:17">
+    <row r="47" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B47" s="7"/>
       <c r="C47" s="7"/>
       <c r="D47" s="7"/>
@@ -10837,7 +10837,7 @@
       <c r="P47" s="7"/>
       <c r="Q47" s="7"/>
     </row>
-    <row r="48" spans="2:17">
+    <row r="48" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B48" s="7"/>
       <c r="C48" s="7"/>
       <c r="D48" s="7"/>
@@ -10859,7 +10859,7 @@
       <c r="P48" s="7"/>
       <c r="Q48" s="7"/>
     </row>
-    <row r="49" spans="2:17">
+    <row r="49" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B49" s="7"/>
       <c r="C49" s="7"/>
       <c r="D49" s="7"/>
@@ -10881,7 +10881,7 @@
       <c r="P49" s="7"/>
       <c r="Q49" s="7"/>
     </row>
-    <row r="50" spans="2:17">
+    <row r="50" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B50" s="7"/>
       <c r="C50" s="7"/>
       <c r="D50" s="7"/>
@@ -10903,7 +10903,7 @@
       <c r="P50" s="7"/>
       <c r="Q50" s="7"/>
     </row>
-    <row r="51" spans="2:17">
+    <row r="51" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B51" s="7"/>
       <c r="C51" s="7"/>
       <c r="D51" s="7"/>
@@ -10925,7 +10925,7 @@
       <c r="P51" s="7"/>
       <c r="Q51" s="7"/>
     </row>
-    <row r="52" spans="2:17">
+    <row r="52" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B52" s="7"/>
       <c r="C52" s="7"/>
       <c r="D52" s="7"/>
@@ -10947,7 +10947,7 @@
       <c r="P52" s="7"/>
       <c r="Q52" s="7"/>
     </row>
-    <row r="53" spans="2:17">
+    <row r="53" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B53" s="7"/>
       <c r="C53" s="7"/>
       <c r="D53" s="7"/>
@@ -10969,7 +10969,7 @@
       <c r="P53" s="7"/>
       <c r="Q53" s="7"/>
     </row>
-    <row r="54" spans="2:17">
+    <row r="54" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B54" s="7"/>
       <c r="C54" s="7"/>
       <c r="D54" s="7"/>
@@ -10991,7 +10991,7 @@
       <c r="P54" s="7"/>
       <c r="Q54" s="7"/>
     </row>
-    <row r="55" spans="2:17">
+    <row r="55" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B55" s="7"/>
       <c r="C55" s="7"/>
       <c r="D55" s="7"/>
@@ -11013,7 +11013,7 @@
       <c r="P55" s="7"/>
       <c r="Q55" s="7"/>
     </row>
-    <row r="56" spans="2:17">
+    <row r="56" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B56" s="7"/>
       <c r="C56" s="7"/>
       <c r="D56" s="7"/>
@@ -11035,7 +11035,7 @@
       <c r="P56" s="7"/>
       <c r="Q56" s="7"/>
     </row>
-    <row r="57" spans="2:17">
+    <row r="57" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B57" s="7"/>
       <c r="C57" s="7"/>
       <c r="D57" s="7"/>
@@ -11057,7 +11057,7 @@
       <c r="P57" s="7"/>
       <c r="Q57" s="7"/>
     </row>
-    <row r="58" spans="2:17">
+    <row r="58" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B58" s="7"/>
       <c r="C58" s="7"/>
       <c r="D58" s="7"/>
@@ -11079,7 +11079,7 @@
       <c r="P58" s="7"/>
       <c r="Q58" s="7"/>
     </row>
-    <row r="59" spans="2:17">
+    <row r="59" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B59" s="7"/>
       <c r="C59" s="7"/>
       <c r="D59" s="7"/>
@@ -11101,7 +11101,7 @@
       <c r="P59" s="7"/>
       <c r="Q59" s="7"/>
     </row>
-    <row r="60" spans="2:17">
+    <row r="60" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B60" s="7"/>
       <c r="C60" s="7"/>
       <c r="D60" s="7"/>
@@ -11123,7 +11123,7 @@
       <c r="P60" s="7"/>
       <c r="Q60" s="7"/>
     </row>
-    <row r="61" spans="2:17">
+    <row r="61" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B61" s="7"/>
       <c r="C61" s="7"/>
       <c r="D61" s="7"/>
@@ -11145,7 +11145,7 @@
       <c r="P61" s="7"/>
       <c r="Q61" s="7"/>
     </row>
-    <row r="62" spans="2:17">
+    <row r="62" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B62" s="7">
         <v>365</v>
       </c>
@@ -11183,7 +11183,7 @@
         <v>44994</v>
       </c>
     </row>
-    <row r="63" spans="2:17">
+    <row r="63" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B63" s="7"/>
       <c r="C63" s="7"/>
       <c r="D63" s="7"/>
@@ -11207,7 +11207,7 @@
       <c r="P63" s="7"/>
       <c r="Q63" s="7"/>
     </row>
-    <row r="64" spans="2:17">
+    <row r="64" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B64" s="7"/>
       <c r="C64" s="7"/>
       <c r="D64" s="7"/>
@@ -11231,7 +11231,7 @@
       <c r="P64" s="7"/>
       <c r="Q64" s="7"/>
     </row>
-    <row r="65" spans="2:17">
+    <row r="65" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B65" s="7"/>
       <c r="C65" s="7"/>
       <c r="D65" s="7"/>
@@ -11255,7 +11255,7 @@
       <c r="P65" s="7"/>
       <c r="Q65" s="7"/>
     </row>
-    <row r="66" spans="2:17">
+    <row r="66" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B66" s="7"/>
       <c r="C66" s="7"/>
       <c r="D66" s="7"/>
@@ -11279,7 +11279,7 @@
       <c r="P66" s="7"/>
       <c r="Q66" s="7"/>
     </row>
-    <row r="67" spans="2:17">
+    <row r="67" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B67" s="7"/>
       <c r="C67" s="7"/>
       <c r="D67" s="7"/>
@@ -11303,7 +11303,7 @@
       <c r="P67" s="7"/>
       <c r="Q67" s="7"/>
     </row>
-    <row r="68" spans="2:17">
+    <row r="68" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B68" s="7"/>
       <c r="C68" s="7"/>
       <c r="D68" s="7"/>
@@ -11327,7 +11327,7 @@
       <c r="P68" s="7"/>
       <c r="Q68" s="7"/>
     </row>
-    <row r="69" spans="2:17">
+    <row r="69" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B69" s="7">
         <v>366</v>
       </c>
@@ -11365,7 +11365,7 @@
         <v>45015</v>
       </c>
     </row>
-    <row r="70" spans="2:17">
+    <row r="70" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B70" s="7"/>
       <c r="C70" s="7"/>
       <c r="D70" s="7"/>
@@ -11389,7 +11389,7 @@
       <c r="P70" s="7"/>
       <c r="Q70" s="7"/>
     </row>
-    <row r="71" spans="2:17">
+    <row r="71" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B71" s="7"/>
       <c r="C71" s="7"/>
       <c r="D71" s="7"/>
@@ -11413,7 +11413,7 @@
       <c r="P71" s="7"/>
       <c r="Q71" s="7"/>
     </row>
-    <row r="72" spans="2:17">
+    <row r="72" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B72" s="7"/>
       <c r="C72" s="7"/>
       <c r="D72" s="7"/>
@@ -11437,7 +11437,7 @@
       <c r="P72" s="7"/>
       <c r="Q72" s="7"/>
     </row>
-    <row r="73" spans="2:17">
+    <row r="73" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B73" s="7"/>
       <c r="C73" s="7"/>
       <c r="D73" s="7"/>
@@ -11461,7 +11461,7 @@
       <c r="P73" s="7"/>
       <c r="Q73" s="7"/>
     </row>
-    <row r="74" spans="2:17">
+    <row r="74" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B74" s="7"/>
       <c r="C74" s="7"/>
       <c r="D74" s="7"/>
@@ -11485,7 +11485,7 @@
       <c r="P74" s="7"/>
       <c r="Q74" s="7"/>
     </row>
-    <row r="75" spans="2:17">
+    <row r="75" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B75" s="7"/>
       <c r="C75" s="7"/>
       <c r="D75" s="7"/>
@@ -11509,7 +11509,7 @@
       <c r="P75" s="7"/>
       <c r="Q75" s="7"/>
     </row>
-    <row r="76" spans="2:17">
+    <row r="76" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B76" s="7">
         <v>367</v>
       </c>
@@ -11547,7 +11547,7 @@
         <v>44994</v>
       </c>
     </row>
-    <row r="77" spans="2:17">
+    <row r="77" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B77" s="7"/>
       <c r="C77" s="7"/>
       <c r="D77" s="7"/>
@@ -11571,7 +11571,7 @@
       <c r="P77" s="7"/>
       <c r="Q77" s="7"/>
     </row>
-    <row r="78" spans="2:17">
+    <row r="78" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B78" s="7"/>
       <c r="C78" s="7"/>
       <c r="D78" s="7"/>
@@ -11595,7 +11595,7 @@
       <c r="P78" s="7"/>
       <c r="Q78" s="7"/>
     </row>
-    <row r="79" spans="2:17">
+    <row r="79" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B79" s="7"/>
       <c r="C79" s="7"/>
       <c r="D79" s="12"/>
@@ -11619,7 +11619,7 @@
       <c r="P79" s="7"/>
       <c r="Q79" s="7"/>
     </row>
-    <row r="80" spans="2:17">
+    <row r="80" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B80" s="7"/>
       <c r="C80" s="7"/>
       <c r="D80" s="12"/>
@@ -11643,7 +11643,7 @@
       <c r="P80" s="7"/>
       <c r="Q80" s="7"/>
     </row>
-    <row r="81" spans="2:17">
+    <row r="81" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B81" s="7"/>
       <c r="C81" s="7"/>
       <c r="D81" s="12"/>
@@ -11667,7 +11667,7 @@
       <c r="P81" s="7"/>
       <c r="Q81" s="7"/>
     </row>
-    <row r="82" spans="2:17">
+    <row r="82" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B82" s="7"/>
       <c r="C82" s="7"/>
       <c r="D82" s="12"/>
@@ -11691,7 +11691,7 @@
       <c r="P82" s="7"/>
       <c r="Q82" s="7"/>
     </row>
-    <row r="83" spans="2:17">
+    <row r="83" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B83" s="7">
         <v>368</v>
       </c>
@@ -11729,7 +11729,7 @@
         <v>45001</v>
       </c>
     </row>
-    <row r="84" spans="2:17">
+    <row r="84" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B84" s="7"/>
       <c r="C84" s="7"/>
       <c r="D84" s="12"/>
@@ -11753,7 +11753,7 @@
       <c r="P84" s="7"/>
       <c r="Q84" s="7"/>
     </row>
-    <row r="85" spans="2:17">
+    <row r="85" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B85" s="7"/>
       <c r="C85" s="7"/>
       <c r="D85" s="12"/>
@@ -11777,7 +11777,7 @@
       <c r="P85" s="7"/>
       <c r="Q85" s="7"/>
     </row>
-    <row r="86" spans="2:17">
+    <row r="86" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B86" s="7"/>
       <c r="C86" s="7"/>
       <c r="D86" s="12"/>
@@ -11801,7 +11801,7 @@
       <c r="P86" s="7"/>
       <c r="Q86" s="7"/>
     </row>
-    <row r="87" spans="2:17">
+    <row r="87" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B87" s="7"/>
       <c r="C87" s="7"/>
       <c r="D87" s="12"/>
@@ -11825,7 +11825,7 @@
       <c r="P87" s="7"/>
       <c r="Q87" s="7"/>
     </row>
-    <row r="88" spans="2:17">
+    <row r="88" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B88" s="7"/>
       <c r="C88" s="7"/>
       <c r="D88" s="12"/>
@@ -11849,7 +11849,7 @@
       <c r="P88" s="7"/>
       <c r="Q88" s="7"/>
     </row>
-    <row r="89" spans="2:17">
+    <row r="89" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B89" s="7"/>
       <c r="C89" s="7"/>
       <c r="D89" s="12"/>
@@ -11873,7 +11873,7 @@
       <c r="P89" s="7"/>
       <c r="Q89" s="7"/>
     </row>
-    <row r="90" spans="2:17">
+    <row r="90" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B90" s="7">
         <v>30008</v>
       </c>
@@ -11907,7 +11907,7 @@
         <v>45015</v>
       </c>
     </row>
-    <row r="91" spans="2:17">
+    <row r="91" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B91" s="7">
         <v>30009</v>
       </c>
@@ -11941,7 +11941,7 @@
         <v>45015</v>
       </c>
     </row>
-    <row r="92" spans="2:17">
+    <row r="92" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B92" s="7">
         <v>30010</v>
       </c>
@@ -11975,7 +11975,7 @@
         <v>45015</v>
       </c>
     </row>
-    <row r="93" spans="2:17">
+    <row r="93" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B93" s="7">
         <v>30011</v>
       </c>
@@ -12009,7 +12009,7 @@
         <v>45015</v>
       </c>
     </row>
-    <row r="94" spans="2:17" ht="54">
+    <row r="94" spans="2:17" ht="54" x14ac:dyDescent="0.3">
       <c r="B94" s="7"/>
       <c r="C94" s="7" t="s">
         <v>315</v>
@@ -12041,7 +12041,7 @@
         <v>45022</v>
       </c>
     </row>
-    <row r="95" spans="2:17">
+    <row r="95" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B95" s="7"/>
       <c r="C95" s="7" t="s">
         <v>315</v>
@@ -12073,7 +12073,7 @@
         <v>45001</v>
       </c>
     </row>
-    <row r="96" spans="2:17">
+    <row r="96" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B96" s="7"/>
       <c r="C96" s="7" t="s">
         <v>315</v>
@@ -12107,7 +12107,7 @@
         <v>45008</v>
       </c>
     </row>
-    <row r="97" spans="2:17" ht="27">
+    <row r="97" spans="2:17" ht="27" x14ac:dyDescent="0.3">
       <c r="B97" s="7"/>
       <c r="C97" s="7" t="s">
         <v>315</v>
@@ -12141,7 +12141,7 @@
         <v>45015</v>
       </c>
     </row>
-    <row r="98" spans="2:17" ht="27">
+    <row r="98" spans="2:17" ht="27" x14ac:dyDescent="0.3">
       <c r="B98" s="7"/>
       <c r="C98" s="7" t="s">
         <v>315</v>
@@ -12175,7 +12175,7 @@
         <v>45022</v>
       </c>
     </row>
-    <row r="99" spans="2:17">
+    <row r="99" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B99" s="7">
         <v>1102</v>
       </c>
@@ -12215,7 +12215,7 @@
         <v>45015</v>
       </c>
     </row>
-    <row r="100" spans="2:17">
+    <row r="100" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B100" s="7"/>
       <c r="C100" s="7"/>
       <c r="D100" s="12"/>
@@ -12237,7 +12237,7 @@
       <c r="P100" s="10"/>
       <c r="Q100" s="10"/>
     </row>
-    <row r="101" spans="2:17">
+    <row r="101" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B101" s="7"/>
       <c r="C101" s="7"/>
       <c r="D101" s="12"/>
@@ -12259,7 +12259,7 @@
       <c r="P101" s="10"/>
       <c r="Q101" s="10"/>
     </row>
-    <row r="102" spans="2:17">
+    <row r="102" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B102" s="7"/>
       <c r="C102" s="7"/>
       <c r="D102" s="12"/>
@@ -12281,7 +12281,7 @@
       <c r="P102" s="10"/>
       <c r="Q102" s="10"/>
     </row>
-    <row r="103" spans="2:17">
+    <row r="103" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B103" s="7"/>
       <c r="C103" s="7"/>
       <c r="D103" s="12"/>
@@ -12303,7 +12303,7 @@
       <c r="P103" s="10"/>
       <c r="Q103" s="10"/>
     </row>
-    <row r="104" spans="2:17">
+    <row r="104" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B104" s="7"/>
       <c r="C104" s="7"/>
       <c r="D104" s="12"/>
@@ -12325,7 +12325,7 @@
       <c r="P104" s="10"/>
       <c r="Q104" s="10"/>
     </row>
-    <row r="105" spans="2:17">
+    <row r="105" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B105" s="7">
         <v>1103</v>
       </c>
@@ -12365,7 +12365,7 @@
         <v>45015</v>
       </c>
     </row>
-    <row r="106" spans="2:17">
+    <row r="106" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B106" s="7"/>
       <c r="C106" s="7"/>
       <c r="D106" s="12"/>
@@ -12387,7 +12387,7 @@
       <c r="P106" s="10"/>
       <c r="Q106" s="10"/>
     </row>
-    <row r="107" spans="2:17">
+    <row r="107" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B107" s="7"/>
       <c r="C107" s="7"/>
       <c r="D107" s="12"/>
@@ -12409,7 +12409,7 @@
       <c r="P107" s="10"/>
       <c r="Q107" s="10"/>
     </row>
-    <row r="108" spans="2:17">
+    <row r="108" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B108" s="7"/>
       <c r="C108" s="7"/>
       <c r="D108" s="12"/>
@@ -12431,7 +12431,7 @@
       <c r="P108" s="10"/>
       <c r="Q108" s="10"/>
     </row>
-    <row r="109" spans="2:17">
+    <row r="109" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B109" s="7"/>
       <c r="C109" s="7"/>
       <c r="D109" s="12"/>
@@ -12453,7 +12453,7 @@
       <c r="P109" s="10"/>
       <c r="Q109" s="10"/>
     </row>
-    <row r="110" spans="2:17">
+    <row r="110" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B110" s="7"/>
       <c r="C110" s="7"/>
       <c r="D110" s="12"/>
@@ -12475,7 +12475,7 @@
       <c r="P110" s="10"/>
       <c r="Q110" s="10"/>
     </row>
-    <row r="111" spans="2:17" ht="27">
+    <row r="111" spans="2:17" ht="27" x14ac:dyDescent="0.3">
       <c r="B111" s="7">
         <v>20007</v>
       </c>
@@ -12511,7 +12511,7 @@
         <v>45015</v>
       </c>
     </row>
-    <row r="112" spans="2:17" ht="27">
+    <row r="112" spans="2:17" ht="27" x14ac:dyDescent="0.3">
       <c r="B112" s="7"/>
       <c r="C112" s="7"/>
       <c r="D112" s="12"/>
@@ -12541,7 +12541,7 @@
         <v>45015</v>
       </c>
     </row>
-    <row r="113" spans="2:17" ht="40.5">
+    <row r="113" spans="2:17" ht="40.5" x14ac:dyDescent="0.3">
       <c r="B113" s="7"/>
       <c r="C113" s="7"/>
       <c r="D113" s="7"/>
@@ -12571,7 +12571,7 @@
         <v>45015</v>
       </c>
     </row>
-    <row r="114" spans="2:17" ht="54">
+    <row r="114" spans="2:17" ht="54" x14ac:dyDescent="0.3">
       <c r="B114" s="7"/>
       <c r="C114" s="7"/>
       <c r="D114" s="7"/>
@@ -12601,7 +12601,7 @@
         <v>45015</v>
       </c>
     </row>
-    <row r="115" spans="2:17" ht="54">
+    <row r="115" spans="2:17" ht="54" x14ac:dyDescent="0.3">
       <c r="B115" s="7"/>
       <c r="C115" s="7"/>
       <c r="D115" s="7"/>
@@ -12631,7 +12631,7 @@
         <v>45015</v>
       </c>
     </row>
-    <row r="116" spans="2:17" ht="54">
+    <row r="116" spans="2:17" ht="54" x14ac:dyDescent="0.3">
       <c r="B116" s="7"/>
       <c r="C116" s="7"/>
       <c r="D116" s="7"/>
@@ -12669,7 +12669,7 @@
       <selection pane="bottomLeft" activeCell="D107" sqref="D107"/>
       <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
       <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
-      <autoFilter ref="B1:Q116" xr:uid="{DC7BFE9A-DA4E-4145-9A61-534ABFE6143C}"/>
+      <autoFilter ref="B1:Q116" xr:uid="{85666439-5170-4EF3-8F29-8CF265646AC5}"/>
     </customSheetView>
   </customSheetViews>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -12687,12 +12687,12 @@
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="E32" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight"/>
+      <selection pane="bottomLeft"/>
       <selection pane="bottomRight" activeCell="E32" sqref="E32"/>
-      <selection pane="bottomLeft"/>
-      <selection pane="topRight"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="10.25" style="34" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.125" style="8" customWidth="1"/>
@@ -12713,7 +12713,7 @@
     <col min="17" max="16384" width="9" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="16.5">
+    <row r="1" spans="1:20" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A1" s="36" t="s">
         <v>0</v>
       </c>
@@ -12767,7 +12767,7 @@
       <c r="S1"/>
       <c r="T1"/>
     </row>
-    <row r="2" spans="1:20" ht="16.5" customHeight="1">
+    <row r="2" spans="1:20" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B2" s="5">
         <v>154</v>
       </c>
@@ -12810,7 +12810,7 @@
       <c r="S2"/>
       <c r="T2"/>
     </row>
-    <row r="3" spans="1:20" ht="16.5">
+    <row r="3" spans="1:20" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B3" s="5"/>
       <c r="C3" s="5"/>
       <c r="D3" s="5"/>
@@ -12839,7 +12839,7 @@
       <c r="S3"/>
       <c r="T3"/>
     </row>
-    <row r="4" spans="1:20" ht="16.5">
+    <row r="4" spans="1:20" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B4" s="5"/>
       <c r="C4" s="5"/>
       <c r="D4" s="5"/>
@@ -12868,7 +12868,7 @@
       <c r="S4"/>
       <c r="T4"/>
     </row>
-    <row r="5" spans="1:20" ht="16.5">
+    <row r="5" spans="1:20" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B5" s="5"/>
       <c r="C5" s="5"/>
       <c r="D5" s="5"/>
@@ -12897,7 +12897,7 @@
       <c r="S5"/>
       <c r="T5"/>
     </row>
-    <row r="6" spans="1:20" ht="16.5">
+    <row r="6" spans="1:20" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
@@ -12926,7 +12926,7 @@
       <c r="S6"/>
       <c r="T6"/>
     </row>
-    <row r="7" spans="1:20" ht="16.5">
+    <row r="7" spans="1:20" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>
       <c r="D7" s="5"/>
@@ -12955,7 +12955,7 @@
       <c r="S7"/>
       <c r="T7"/>
     </row>
-    <row r="8" spans="1:20" ht="16.5">
+    <row r="8" spans="1:20" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B8" s="5"/>
       <c r="C8" s="5"/>
       <c r="D8" s="5"/>
@@ -12984,7 +12984,7 @@
       <c r="S8"/>
       <c r="T8"/>
     </row>
-    <row r="9" spans="1:20" ht="16.5">
+    <row r="9" spans="1:20" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B9" s="5"/>
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
@@ -13013,7 +13013,7 @@
       <c r="S9"/>
       <c r="T9"/>
     </row>
-    <row r="10" spans="1:20" ht="16.5">
+    <row r="10" spans="1:20" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B10" s="5"/>
       <c r="C10" s="5"/>
       <c r="D10" s="5"/>
@@ -13042,7 +13042,7 @@
       <c r="S10"/>
       <c r="T10"/>
     </row>
-    <row r="11" spans="1:20" ht="16.5">
+    <row r="11" spans="1:20" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B11" s="7"/>
       <c r="C11" s="7"/>
       <c r="D11" s="7"/>
@@ -13071,7 +13071,7 @@
       <c r="S11"/>
       <c r="T11"/>
     </row>
-    <row r="12" spans="1:20" s="20" customFormat="1" ht="16.5">
+    <row r="12" spans="1:20" s="20" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A12" s="34"/>
       <c r="B12" s="21">
         <v>155</v>
@@ -13115,7 +13115,7 @@
       <c r="S12" s="25"/>
       <c r="T12" s="25"/>
     </row>
-    <row r="13" spans="1:20" s="20" customFormat="1" ht="16.5">
+    <row r="13" spans="1:20" s="20" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A13" s="34"/>
       <c r="B13" s="21"/>
       <c r="C13" s="22"/>
@@ -13145,7 +13145,7 @@
       <c r="S13" s="25"/>
       <c r="T13" s="25"/>
     </row>
-    <row r="14" spans="1:20" s="20" customFormat="1" ht="16.5">
+    <row r="14" spans="1:20" s="20" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A14" s="34"/>
       <c r="B14" s="21"/>
       <c r="C14" s="22"/>
@@ -13175,7 +13175,7 @@
       <c r="S14" s="25"/>
       <c r="T14" s="25"/>
     </row>
-    <row r="15" spans="1:20" s="20" customFormat="1" ht="16.5">
+    <row r="15" spans="1:20" s="20" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A15" s="34"/>
       <c r="B15" s="21"/>
       <c r="C15" s="22"/>
@@ -13205,7 +13205,7 @@
       <c r="S15" s="25"/>
       <c r="T15" s="25"/>
     </row>
-    <row r="16" spans="1:20" s="20" customFormat="1" ht="16.5">
+    <row r="16" spans="1:20" s="20" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A16" s="34"/>
       <c r="B16" s="21"/>
       <c r="C16" s="22"/>
@@ -13235,7 +13235,7 @@
       <c r="S16" s="25"/>
       <c r="T16" s="25"/>
     </row>
-    <row r="17" spans="1:20" s="20" customFormat="1" ht="16.5">
+    <row r="17" spans="1:20" s="20" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A17" s="34"/>
       <c r="B17" s="21"/>
       <c r="C17" s="22"/>
@@ -13265,7 +13265,7 @@
       <c r="S17" s="25"/>
       <c r="T17" s="25"/>
     </row>
-    <row r="18" spans="1:20" s="20" customFormat="1" ht="16.5">
+    <row r="18" spans="1:20" s="20" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A18" s="34"/>
       <c r="B18" s="21"/>
       <c r="C18" s="22"/>
@@ -13295,7 +13295,7 @@
       <c r="S18" s="25"/>
       <c r="T18" s="25"/>
     </row>
-    <row r="19" spans="1:20" s="20" customFormat="1" ht="16.5">
+    <row r="19" spans="1:20" s="20" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A19" s="34"/>
       <c r="B19" s="21"/>
       <c r="C19" s="22"/>
@@ -13325,7 +13325,7 @@
       <c r="S19" s="25"/>
       <c r="T19" s="25"/>
     </row>
-    <row r="20" spans="1:20" s="20" customFormat="1" ht="16.5">
+    <row r="20" spans="1:20" s="20" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A20" s="34"/>
       <c r="B20" s="21"/>
       <c r="C20" s="22"/>
@@ -13355,7 +13355,7 @@
       <c r="S20" s="25"/>
       <c r="T20" s="25"/>
     </row>
-    <row r="21" spans="1:20" s="20" customFormat="1" ht="16.5">
+    <row r="21" spans="1:20" s="20" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A21" s="34"/>
       <c r="B21" s="21"/>
       <c r="C21" s="22"/>
@@ -13385,7 +13385,7 @@
       <c r="S21" s="25"/>
       <c r="T21" s="25"/>
     </row>
-    <row r="22" spans="1:20" ht="16.5">
+    <row r="22" spans="1:20" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B22" s="7">
         <v>372</v>
       </c>
@@ -13430,7 +13430,7 @@
       <c r="S22"/>
       <c r="T22"/>
     </row>
-    <row r="23" spans="1:20" ht="16.5">
+    <row r="23" spans="1:20" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B23" s="7"/>
       <c r="C23" s="5"/>
       <c r="D23" s="7"/>
@@ -13461,7 +13461,7 @@
       <c r="S23"/>
       <c r="T23"/>
     </row>
-    <row r="24" spans="1:20" ht="16.5">
+    <row r="24" spans="1:20" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B24" s="7"/>
       <c r="C24" s="5"/>
       <c r="D24" s="7"/>
@@ -13492,7 +13492,7 @@
       <c r="S24"/>
       <c r="T24"/>
     </row>
-    <row r="25" spans="1:20" ht="16.5">
+    <row r="25" spans="1:20" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B25" s="7"/>
       <c r="C25" s="5"/>
       <c r="D25" s="7"/>
@@ -13523,7 +13523,7 @@
       <c r="S25"/>
       <c r="T25"/>
     </row>
-    <row r="26" spans="1:20" ht="16.5">
+    <row r="26" spans="1:20" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B26" s="7"/>
       <c r="C26" s="5"/>
       <c r="D26" s="7"/>
@@ -13554,7 +13554,7 @@
       <c r="S26"/>
       <c r="T26"/>
     </row>
-    <row r="27" spans="1:20" ht="16.5">
+    <row r="27" spans="1:20" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B27" s="7"/>
       <c r="C27" s="5"/>
       <c r="D27" s="7"/>
@@ -13585,7 +13585,7 @@
       <c r="S27"/>
       <c r="T27"/>
     </row>
-    <row r="28" spans="1:20" ht="16.5">
+    <row r="28" spans="1:20" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B28" s="7"/>
       <c r="C28" s="5"/>
       <c r="D28" s="7"/>
@@ -13616,7 +13616,7 @@
       <c r="S28"/>
       <c r="T28"/>
     </row>
-    <row r="29" spans="1:20" s="20" customFormat="1" ht="16.5">
+    <row r="29" spans="1:20" s="20" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A29" s="34"/>
       <c r="B29" s="21">
         <v>373</v>
@@ -13662,7 +13662,7 @@
       <c r="S29" s="25"/>
       <c r="T29" s="25"/>
     </row>
-    <row r="30" spans="1:20" s="20" customFormat="1" ht="16.5">
+    <row r="30" spans="1:20" s="20" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A30" s="34"/>
       <c r="B30" s="21"/>
       <c r="C30" s="22"/>
@@ -13694,7 +13694,7 @@
       <c r="S30" s="25"/>
       <c r="T30" s="25"/>
     </row>
-    <row r="31" spans="1:20" s="20" customFormat="1" ht="16.5">
+    <row r="31" spans="1:20" s="20" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A31" s="34"/>
       <c r="B31" s="21"/>
       <c r="C31" s="21"/>
@@ -13726,7 +13726,7 @@
       <c r="S31" s="25"/>
       <c r="T31" s="25"/>
     </row>
-    <row r="32" spans="1:20" s="20" customFormat="1" ht="16.5">
+    <row r="32" spans="1:20" s="20" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A32" s="34"/>
       <c r="B32" s="21"/>
       <c r="C32" s="21"/>
@@ -13758,7 +13758,7 @@
       <c r="S32" s="25"/>
       <c r="T32" s="25"/>
     </row>
-    <row r="33" spans="1:20" s="20" customFormat="1" ht="16.5">
+    <row r="33" spans="1:20" s="20" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A33" s="34"/>
       <c r="B33" s="21"/>
       <c r="C33" s="21"/>
@@ -13790,7 +13790,7 @@
       <c r="S33" s="25"/>
       <c r="T33" s="25"/>
     </row>
-    <row r="34" spans="1:20" s="20" customFormat="1" ht="16.5">
+    <row r="34" spans="1:20" s="20" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A34" s="34"/>
       <c r="B34" s="21"/>
       <c r="C34" s="21"/>
@@ -13822,7 +13822,7 @@
       <c r="S34" s="25"/>
       <c r="T34" s="25"/>
     </row>
-    <row r="35" spans="1:20" s="20" customFormat="1" ht="16.5">
+    <row r="35" spans="1:20" s="20" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A35" s="34"/>
       <c r="B35" s="21"/>
       <c r="C35" s="21"/>
@@ -13854,7 +13854,7 @@
       <c r="S35" s="25"/>
       <c r="T35" s="25"/>
     </row>
-    <row r="36" spans="1:20" ht="16.5">
+    <row r="36" spans="1:20" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B36" s="7">
         <v>30013</v>
       </c>
@@ -13893,7 +13893,7 @@
       <c r="S36"/>
       <c r="T36"/>
     </row>
-    <row r="37" spans="1:20" s="20" customFormat="1" ht="16.5">
+    <row r="37" spans="1:20" s="20" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A37" s="34"/>
       <c r="B37" s="21">
         <v>20009</v>
@@ -13935,7 +13935,7 @@
       <c r="S37" s="25"/>
       <c r="T37" s="25"/>
     </row>
-    <row r="38" spans="1:20" s="20" customFormat="1" ht="16.5">
+    <row r="38" spans="1:20" s="20" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A38" s="34"/>
       <c r="B38" s="21"/>
       <c r="C38" s="21"/>
@@ -13965,7 +13965,7 @@
       <c r="S38" s="25"/>
       <c r="T38" s="25"/>
     </row>
-    <row r="39" spans="1:20" s="20" customFormat="1" ht="16.5">
+    <row r="39" spans="1:20" s="20" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A39" s="34"/>
       <c r="B39" s="21"/>
       <c r="C39" s="21"/>
@@ -13995,7 +13995,7 @@
       <c r="S39" s="25"/>
       <c r="T39" s="25"/>
     </row>
-    <row r="40" spans="1:20" s="20" customFormat="1" ht="16.5">
+    <row r="40" spans="1:20" s="20" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A40" s="34"/>
       <c r="B40" s="21"/>
       <c r="C40" s="21"/>
@@ -14025,7 +14025,7 @@
       <c r="S40" s="25"/>
       <c r="T40" s="25"/>
     </row>
-    <row r="41" spans="1:20" s="20" customFormat="1" ht="16.5">
+    <row r="41" spans="1:20" s="20" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A41" s="34"/>
       <c r="B41" s="21"/>
       <c r="C41" s="21"/>
@@ -14055,7 +14055,7 @@
       <c r="S41" s="25"/>
       <c r="T41" s="25"/>
     </row>
-    <row r="42" spans="1:20" s="20" customFormat="1" ht="16.5">
+    <row r="42" spans="1:20" s="20" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A42" s="34"/>
       <c r="B42" s="21"/>
       <c r="C42" s="21"/>
@@ -14085,7 +14085,7 @@
       <c r="S42" s="25"/>
       <c r="T42" s="25"/>
     </row>
-    <row r="43" spans="1:20" s="20" customFormat="1" ht="16.5">
+    <row r="43" spans="1:20" s="20" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A43" s="34"/>
       <c r="B43" s="21"/>
       <c r="C43" s="21"/>
@@ -14115,7 +14115,7 @@
       <c r="S43" s="25"/>
       <c r="T43" s="25"/>
     </row>
-    <row r="44" spans="1:20" s="20" customFormat="1" ht="16.5">
+    <row r="44" spans="1:20" s="20" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A44" s="34"/>
       <c r="B44" s="21"/>
       <c r="C44" s="21"/>
@@ -14145,7 +14145,7 @@
       <c r="S44" s="25"/>
       <c r="T44" s="25"/>
     </row>
-    <row r="45" spans="1:20" s="20" customFormat="1" ht="16.5">
+    <row r="45" spans="1:20" s="20" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A45" s="34"/>
       <c r="B45" s="21"/>
       <c r="C45" s="21"/>
@@ -14175,7 +14175,7 @@
       <c r="S45" s="25"/>
       <c r="T45" s="25"/>
     </row>
-    <row r="46" spans="1:20" ht="16.5">
+    <row r="46" spans="1:20" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B46" s="7">
         <v>1106</v>
       </c>
@@ -14214,7 +14214,7 @@
       <c r="S46"/>
       <c r="T46"/>
     </row>
-    <row r="47" spans="1:20" ht="16.5">
+    <row r="47" spans="1:20" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B47" s="7"/>
       <c r="C47" s="7"/>
       <c r="D47" s="12"/>
@@ -14239,7 +14239,7 @@
       <c r="S47"/>
       <c r="T47"/>
     </row>
-    <row r="48" spans="1:20" ht="16.5">
+    <row r="48" spans="1:20" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B48" s="7"/>
       <c r="C48" s="7"/>
       <c r="D48" s="12"/>
@@ -14264,7 +14264,7 @@
       <c r="S48"/>
       <c r="T48"/>
     </row>
-    <row r="49" spans="1:20" ht="16.5">
+    <row r="49" spans="1:20" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B49" s="7"/>
       <c r="C49" s="7"/>
       <c r="D49" s="12"/>
@@ -14289,7 +14289,7 @@
       <c r="S49"/>
       <c r="T49"/>
     </row>
-    <row r="50" spans="1:20" ht="16.5">
+    <row r="50" spans="1:20" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B50" s="7"/>
       <c r="C50" s="7"/>
       <c r="D50" s="12"/>
@@ -14314,7 +14314,7 @@
       <c r="S50"/>
       <c r="T50"/>
     </row>
-    <row r="51" spans="1:20" ht="16.5">
+    <row r="51" spans="1:20" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B51" s="7"/>
       <c r="C51" s="7"/>
       <c r="D51" s="12"/>
@@ -14339,7 +14339,7 @@
       <c r="S51"/>
       <c r="T51"/>
     </row>
-    <row r="52" spans="1:20" ht="16.5">
+    <row r="52" spans="1:20" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B52" s="7"/>
       <c r="C52" s="7"/>
       <c r="D52" s="12"/>
@@ -14364,7 +14364,7 @@
       <c r="S52"/>
       <c r="T52"/>
     </row>
-    <row r="53" spans="1:20" s="20" customFormat="1" ht="16.5">
+    <row r="53" spans="1:20" s="20" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A53" s="34"/>
       <c r="B53" s="21">
         <v>1107</v>
@@ -14404,7 +14404,7 @@
       <c r="S53" s="25"/>
       <c r="T53" s="25"/>
     </row>
-    <row r="54" spans="1:20" s="20" customFormat="1" ht="16.5">
+    <row r="54" spans="1:20" s="20" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A54" s="34"/>
       <c r="B54" s="21"/>
       <c r="C54" s="21"/>
@@ -14430,7 +14430,7 @@
       <c r="S54" s="25"/>
       <c r="T54" s="25"/>
     </row>
-    <row r="55" spans="1:20" s="20" customFormat="1" ht="16.5">
+    <row r="55" spans="1:20" s="20" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A55" s="34"/>
       <c r="B55" s="21"/>
       <c r="C55" s="21"/>
@@ -14456,7 +14456,7 @@
       <c r="S55" s="25"/>
       <c r="T55" s="25"/>
     </row>
-    <row r="56" spans="1:20" s="20" customFormat="1" ht="16.5">
+    <row r="56" spans="1:20" s="20" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A56" s="34"/>
       <c r="B56" s="21"/>
       <c r="C56" s="21"/>
@@ -14482,7 +14482,7 @@
       <c r="S56" s="25"/>
       <c r="T56" s="25"/>
     </row>
-    <row r="57" spans="1:20" s="20" customFormat="1" ht="16.5">
+    <row r="57" spans="1:20" s="20" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A57" s="34"/>
       <c r="B57" s="21"/>
       <c r="C57" s="21"/>
@@ -14508,7 +14508,7 @@
       <c r="S57" s="25"/>
       <c r="T57" s="25"/>
     </row>
-    <row r="58" spans="1:20" s="20" customFormat="1" ht="16.5">
+    <row r="58" spans="1:20" s="20" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A58" s="34"/>
       <c r="B58" s="21"/>
       <c r="C58" s="21"/>
@@ -14543,15 +14543,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="문서" ma:contentTypeID="0x010100035D89899FF2E144AC5CDF3E0C05E410" ma:contentTypeVersion="13" ma:contentTypeDescription="새 문서를 만듭니다." ma:contentTypeScope="" ma:versionID="c9fd8eca086ce0b1d107e2b3545271c5">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="7b850dbe-2bbc-4312-b635-0ac631df3b32" xmlns:ns3="1e91ce72-769a-45b6-b2e9-1e3503954573" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="32feda35c5f9fbcce1e6de1bd5c59630" ns2:_="" ns3:_="">
     <xsd:import namespace="7b850dbe-2bbc-4312-b635-0ac631df3b32"/>
@@ -14774,10 +14765,38 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{171D66FE-42B9-4914-A8C9-E322ECCEF2B0}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{20D6D224-8B4D-4E37-8696-12F3450EDE0B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="7b850dbe-2bbc-4312-b635-0ac631df3b32"/>
+    <ds:schemaRef ds:uri="1e91ce72-769a-45b6-b2e9-1e3503954573"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{20D6D224-8B4D-4E37-8696-12F3450EDE0B}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{171D66FE-42B9-4914-A8C9-E322ECCEF2B0}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>